<commit_message>
Fixed Excel test cases file.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\BackTesting Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7755465C-83BE-4C67-B9AE-8F3F4ED08FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ACAFB1-679D-4728-9839-BB5F5A876B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Interval Possible Values: 1 3 5 15 30 60 120 240 360 720 "D" "W"</t>
+          <t>Interval Possible Values: 1, 3, 5, 15, 30, 60, 120, 240, 360, 720, D, W</t>
         </r>
       </text>
     </comment>
@@ -95,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -155,10 +155,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,7 +444,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Replaced max num consecutive (long, short) by (win, loss) in the statistics.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ACAFB1-679D-4728-9839-BB5F5A876B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CD88D4-D6A3-4861-AB51-7FB78D54B114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Symbol</t>
   </si>
@@ -78,16 +78,7 @@
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>BTCUSD</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>Test_Num</t>
-  </si>
-  <si>
-    <t>ETHUSDT</t>
   </si>
 </sst>
 </file>
@@ -441,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +452,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -514,64 +505,6 @@
         <v>1</v>
       </c>
       <c r="I2" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6">
-        <v>43101</v>
-      </c>
-      <c r="D3" s="6">
-        <v>44530</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6">
-        <v>44197</v>
-      </c>
-      <c r="D4" s="6">
-        <v>44531</v>
-      </c>
-      <c r="E4" s="3">
-        <v>60</v>
-      </c>
-      <c r="F4" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G4" s="3">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added win/loose index in the statistics and shifted trade entries by +1.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CD88D4-D6A3-4861-AB51-7FB78D54B114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC5B58-9005-48DB-BDD9-41D2443DD0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,7 +499,7 @@
         <v>10000</v>
       </c>
       <c r="G2" s="3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H2" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
Replaces the console stats output by Excel file output.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEC5B58-9005-48DB-BDD9-41D2443DD0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1719244-C087-4A8C-A73C-2AFA12035750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Symbol</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Test_Num</t>
+  </si>
+  <si>
+    <t>ETHUSD</t>
+  </si>
+  <si>
+    <t>DOTUSDT</t>
+  </si>
+  <si>
+    <t>BTCUSD</t>
+  </si>
+  <si>
+    <t>ADAUSDT</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,6 +520,122 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44378</v>
+      </c>
+      <c r="D3" s="6">
+        <v>44561</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6">
+        <v>44378</v>
+      </c>
+      <c r="D4" s="6">
+        <v>44561</v>
+      </c>
+      <c r="E4" s="3">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6">
+        <v>44378</v>
+      </c>
+      <c r="D5" s="6">
+        <v>44561</v>
+      </c>
+      <c r="E5" s="3">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44378</v>
+      </c>
+      <c r="D6" s="6">
+        <v>44561</v>
+      </c>
+      <c r="E6" s="3">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Plit fees into maker/taker and convert take profits to maker orders.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTestingTradingStrategies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A57477-2DBF-420A-B7E8-9FA75EB8DE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C370C9CA-7AE7-497D-992E-25FADABE97B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ListOfValues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,71 +25,57 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Seb</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{4E80EB13-8DA3-4FAA-98B9-FAE3D2490073}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Interval Possible Values: 1, 3, 5, 15, 30, 60, 120, 240, 360, 720, D, W</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Symbol</t>
   </si>
   <si>
-    <t>From_Time</t>
-  </si>
-  <si>
-    <t>To_Time</t>
-  </si>
-  <si>
     <t>Interval</t>
   </si>
   <si>
-    <t>Trade_Amount</t>
-  </si>
-  <si>
-    <t>Take_Profit_PCT</t>
-  </si>
-  <si>
-    <t>Stop_Loss_PCT</t>
-  </si>
-  <si>
-    <t>Fees_PCT</t>
-  </si>
-  <si>
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>Test_Num</t>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Trade Amount</t>
+  </si>
+  <si>
+    <t>TP %</t>
+  </si>
+  <si>
+    <t>SL %</t>
+  </si>
+  <si>
+    <t>Maker Fee %</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Taker Fee %</t>
+  </si>
+  <si>
+    <t>Test #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,23 +91,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -128,28 +114,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -431,86 +441,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="A3:I6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="11.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="3"/>
-    <col min="6" max="6" width="14.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>44470</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>44530</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>30</v>
       </c>
       <c r="F2" s="3">
         <v>10000</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>1.5</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="1">
         <v>1</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="1">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="J2" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Interval" prompt="Please select value from dropdown" xr:uid="{84749C17-2E54-48BF-AEA9-0BF0C7B46C4A}">
+          <x14:formula1>
+            <xm:f>ListOfValues!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E116</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183ECDD1-3B17-49FC-A8D8-202F644155E1}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added caching data feature for exchanges.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4BD624-3C02-414E-9065-C8E326738B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB63925-B311-4A71-A2E3-2906D76E829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>MACD</t>
   </si>
   <si>
-    <t>Early MACD</t>
-  </si>
-  <si>
     <t>Binance</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>ETHUSDT</t>
+  </si>
+  <si>
+    <t>EarlyMACD</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,10 +569,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4">
         <v>44440</v>
@@ -607,10 +607,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>44440</v>
@@ -675,7 +675,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +702,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>19</v>
@@ -719,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" s="9">
         <v>3</v>

</xml_diff>

<commit_message>
Renamed GT_ema200 column to 'trend' in MACD and EarlyMACD strategies.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB63925-B311-4A71-A2E3-2906D76E829C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5039D9F-0B49-4F7B-9E75-54AFC8B2561D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tweaked indicator calculation for MACD and EarlyMACD.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5039D9F-0B49-4F7B-9E75-54AFC8B2561D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A511B885-2579-4A1B-A1E4-E829661D1345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="492" yWindow="0" windowWidth="21804" windowHeight="6564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tweaked indicator calculation for EarlyMACD.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A511B885-2579-4A1B-A1E4-E829661D1345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DD0105-21C6-4A32-A4FC-A9782BE47FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="492" yWindow="0" windowWidth="21804" windowHeight="6564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +599,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -637,7 +637,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized csv file mode.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DD0105-21C6-4A32-A4FC-A9782BE47FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7E6BB5-287E-4F22-B6D4-04AD02AA801C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="492" yWindow="0" windowWidth="21804" windowHeight="6564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Symbol</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>BTCUSDT</t>
-  </si>
-  <si>
-    <t>ETHUSDT</t>
   </si>
   <si>
     <t>EarlyMACD</t>
@@ -509,7 +506,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,10 +572,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="4">
-        <v>44440</v>
+        <v>44197</v>
       </c>
       <c r="E2" s="4">
-        <v>44550</v>
+        <v>44555</v>
       </c>
       <c r="F2" s="1">
         <v>30</v>
@@ -599,7 +596,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -607,16 +604,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4">
-        <v>44440</v>
+        <v>44197</v>
       </c>
       <c r="E3" s="4">
-        <v>44550</v>
+        <v>44555</v>
       </c>
       <c r="F3" s="1">
         <v>30</v>
@@ -637,7 +634,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +716,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="9">
         <v>3</v>

</xml_diff>

<commit_message>
Added execution time for each test.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7E6BB5-287E-4F22-B6D4-04AD02AA801C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A249503-AA23-4686-A4B9-49BE0BCA9846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,7 +572,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="4">
-        <v>44197</v>
+        <v>40179</v>
       </c>
       <c r="E2" s="4">
         <v>44555</v>
@@ -610,7 +610,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="4">
-        <v>44197</v>
+        <v>40179</v>
       </c>
       <c r="E3" s="4">
         <v>44555</v>

</xml_diff>

<commit_message>
Changed trade entry to limit order.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A249503-AA23-4686-A4B9-49BE0BCA9846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C495A71-060A-4AE0-9004-EF18F68E7501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,10 +572,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="4">
-        <v>40179</v>
+        <v>44470</v>
       </c>
       <c r="E2" s="4">
-        <v>44555</v>
+        <v>44561</v>
       </c>
       <c r="F2" s="1">
         <v>30</v>
@@ -584,10 +584,10 @@
         <v>10000</v>
       </c>
       <c r="H2" s="10">
-        <v>1.5</v>
+        <v>9</v>
       </c>
       <c r="I2" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" s="15">
         <v>-2.5000000000000001E-2</v>
@@ -596,7 +596,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -604,16 +604,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="4">
-        <v>40179</v>
+        <v>44470</v>
       </c>
       <c r="E3" s="4">
-        <v>44555</v>
+        <v>44561</v>
       </c>
       <c r="F3" s="1">
         <v>30</v>
@@ -622,10 +622,10 @@
         <v>10000</v>
       </c>
       <c r="H3" s="10">
-        <v>1.5</v>
+        <v>9</v>
       </c>
       <c r="I3" s="10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J3" s="15">
         <v>-2.5000000000000001E-2</v>

</xml_diff>

<commit_message>
Rounded results in Statistics file.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C495A71-060A-4AE0-9004-EF18F68E7501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8949A26C-4EAC-4D39-9236-3201F013AEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Symbol</t>
   </si>
@@ -101,8 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -176,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,44 +183,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,58 +503,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.21875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" style="10" customWidth="1"/>
-    <col min="8" max="8" width="8" style="10" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" style="10" customWidth="1"/>
-    <col min="10" max="11" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="8" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -562,79 +562,41 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4">
-        <v>44470</v>
-      </c>
-      <c r="E2" s="4">
-        <v>44561</v>
+      <c r="D2" s="14">
+        <v>42972</v>
+      </c>
+      <c r="E2" s="14">
+        <v>44550</v>
       </c>
       <c r="F2" s="1">
         <v>30</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="8">
         <v>10000</v>
       </c>
-      <c r="H2" s="10">
-        <v>9</v>
-      </c>
-      <c r="I2" s="10">
-        <v>6</v>
-      </c>
-      <c r="J2" s="15">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="J2" s="13">
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="13">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="4">
-        <v>44470</v>
-      </c>
-      <c r="E3" s="4">
-        <v>44561</v>
-      </c>
-      <c r="F3" s="1">
-        <v>30</v>
-      </c>
-      <c r="G3" s="10">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="10">
-        <v>9</v>
-      </c>
-      <c r="I3" s="10">
-        <v>6</v>
-      </c>
-      <c r="J3" s="15">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="K3" s="15">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -684,106 +646,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>3</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9">
+      <c r="A4" s="11"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7">
         <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7">
         <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7">
         <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7">
         <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed maker/taker fees from params and moved them into the exchange classes.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8949A26C-4EAC-4D39-9236-3201F013AEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4105825-8F82-4E79-90DE-5A850FFD3A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1032" yWindow="984" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
-  <si>
-    <t>Symbol</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Interval</t>
   </si>
@@ -49,18 +46,6 @@
     <t>SL %</t>
   </si>
   <si>
-    <t>Maker Fee %</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Taker Fee %</t>
-  </si>
-  <si>
     <t>Test #</t>
   </si>
   <si>
@@ -95,15 +80,51 @@
   </si>
   <si>
     <t>EarlyMACD</t>
+  </si>
+  <si>
+    <t>Pair</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>5m</t>
+  </si>
+  <si>
+    <t>15m</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>1w</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,18 +231,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,89 +535,107 @@
     <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.21875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.5546875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="8" style="8" customWidth="1"/>
-    <col min="9" max="9" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="6.88671875" style="16" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="14">
-        <v>42972</v>
-      </c>
-      <c r="E2" s="14">
-        <v>44550</v>
-      </c>
-      <c r="F2" s="1">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="12">
+        <v>44440</v>
+      </c>
+      <c r="E2" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="J2" s="13">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="K2" s="13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
+      <c r="H2" s="16">
+        <v>9</v>
+      </c>
+      <c r="I2" s="16">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="12">
+        <v>44440</v>
+      </c>
+      <c r="E3" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="16">
+        <v>9</v>
+      </c>
+      <c r="I3" s="16">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -615,7 +654,7 @@
           <x14:formula1>
             <xm:f>ListOfValues!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Interval" prompt="Please select interval from dropdown list" xr:uid="{B01186AF-2E82-4CE1-BAFD-D7EED7D3D148}">
           <x14:formula1>
@@ -634,7 +673,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,106 +686,106 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="7">
-        <v>3</v>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="7">
-        <v>5</v>
+      <c r="C4" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="7">
-        <v>15</v>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
-      <c r="C6" s="7">
-        <v>30</v>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
-      <c r="C7" s="7">
-        <v>60</v>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
-      <c r="C8" s="7">
-        <v>120</v>
+      <c r="C8" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
-      <c r="C9" s="7">
-        <v>240</v>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
-      <c r="C10" s="7">
-        <v>360</v>
+      <c r="C10" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
-      <c r="C11" s="7">
-        <v>720</v>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed column TradeAmount to InitalCapital.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4105825-8F82-4E79-90DE-5A850FFD3A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D274E896-C6DE-4722-AE90-0412884E3FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1032" yWindow="984" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>To</t>
   </si>
   <si>
-    <t>Trade Amount</t>
-  </si>
-  <si>
     <t>TP %</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>1w</t>
+  </si>
+  <si>
+    <t>Initial Capital</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,20 +537,20 @@
     <col min="3" max="3" width="11.21875" style="1" customWidth="1"/>
     <col min="4" max="5" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6.88671875" style="16" customWidth="1"/>
     <col min="10" max="10" width="13.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>1</v>
@@ -562,16 +562,16 @@
         <v>0</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -579,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="12">
         <v>44440</v>
@@ -591,7 +591,7 @@
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -603,7 +603,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -611,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="12">
         <v>44440</v>
@@ -623,7 +623,7 @@
         <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
@@ -635,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -686,106 +686,106 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed format of execution time.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99F1E00-3C88-46E8-A3DE-A4C7DB3FCC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57013416-244D-400A-8DB3-E09F593BDC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1728" yWindow="1680" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Initial Capital</t>
+  </si>
+  <si>
+    <t>Scalping1</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,6 +247,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,13 +589,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44440</v>
+        <v>44470</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -611,19 +615,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44440</v>
+        <v>44470</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
@@ -637,6 +641,1682 @@
       <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12">
+        <v>44470</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="17"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="17"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="17"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="17"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="17"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="17"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="17"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="17"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="17"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="17"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="17"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="17"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="17"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="17"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="17"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="17"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="17"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="17"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="17"/>
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="17"/>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="17"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
+      <c r="F61"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="17"/>
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
+      <c r="F62"/>
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="17"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63"/>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="17"/>
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64"/>
+      <c r="H64"/>
+      <c r="I64"/>
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="17"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="17"/>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="17"/>
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="17"/>
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+      <c r="J68"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="17"/>
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69"/>
+      <c r="H69"/>
+      <c r="I69"/>
+      <c r="J69"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="17"/>
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="17"/>
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="17"/>
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="17"/>
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73"/>
+      <c r="I73"/>
+      <c r="J73"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="17"/>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+      <c r="H74"/>
+      <c r="I74"/>
+      <c r="J74"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="17"/>
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+      <c r="H75"/>
+      <c r="I75"/>
+      <c r="J75"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="17"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+      <c r="J76"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="17"/>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+      <c r="J77"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="17"/>
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="17"/>
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79"/>
+      <c r="J79"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="17"/>
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="17"/>
+      <c r="B81"/>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+      <c r="J81"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="17"/>
+      <c r="B82"/>
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+      <c r="J82"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="17"/>
+      <c r="B83"/>
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+      <c r="J83"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="17"/>
+      <c r="B84"/>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+      <c r="J84"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="17"/>
+      <c r="B85"/>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+      <c r="J85"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="17"/>
+      <c r="B86"/>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+      <c r="J86"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="17"/>
+      <c r="B87"/>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+      <c r="J87"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="17"/>
+      <c r="B88"/>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+      <c r="J88"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="17"/>
+      <c r="B89"/>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+      <c r="J89"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="17"/>
+      <c r="B90"/>
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+      <c r="J90"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="17"/>
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+      <c r="J91"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="17"/>
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+      <c r="J92"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="17"/>
+      <c r="B93"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
+      <c r="J93"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="17"/>
+      <c r="B94"/>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
+      <c r="J94"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="17"/>
+      <c r="B95"/>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+      <c r="J95"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="17"/>
+      <c r="B96"/>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+      <c r="J96"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="17"/>
+      <c r="B97"/>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="G97"/>
+      <c r="H97"/>
+      <c r="I97"/>
+      <c r="J97"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="17"/>
+      <c r="B98"/>
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="G98"/>
+      <c r="H98"/>
+      <c r="I98"/>
+      <c r="J98"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="17"/>
+      <c r="B99"/>
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="G99"/>
+      <c r="H99"/>
+      <c r="I99"/>
+      <c r="J99"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="17"/>
+      <c r="B100"/>
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+      <c r="H100"/>
+      <c r="I100"/>
+      <c r="J100"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="17"/>
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
+      <c r="J101"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="17"/>
+      <c r="B102"/>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
+      <c r="J102"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="17"/>
+      <c r="B103"/>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="G103"/>
+      <c r="H103"/>
+      <c r="I103"/>
+      <c r="J103"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="17"/>
+      <c r="B104"/>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104"/>
+      <c r="F104"/>
+      <c r="G104"/>
+      <c r="H104"/>
+      <c r="I104"/>
+      <c r="J104"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="17"/>
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105"/>
+      <c r="F105"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+      <c r="J105"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106" s="17"/>
+      <c r="B106"/>
+      <c r="C106"/>
+      <c r="D106"/>
+      <c r="E106"/>
+      <c r="F106"/>
+      <c r="G106"/>
+      <c r="H106"/>
+      <c r="I106"/>
+      <c r="J106"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107" s="17"/>
+      <c r="B107"/>
+      <c r="C107"/>
+      <c r="D107"/>
+      <c r="E107"/>
+      <c r="F107"/>
+      <c r="G107"/>
+      <c r="H107"/>
+      <c r="I107"/>
+      <c r="J107"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108" s="17"/>
+      <c r="B108"/>
+      <c r="C108"/>
+      <c r="D108"/>
+      <c r="E108"/>
+      <c r="F108"/>
+      <c r="G108"/>
+      <c r="H108"/>
+      <c r="I108"/>
+      <c r="J108"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109" s="17"/>
+      <c r="B109"/>
+      <c r="C109"/>
+      <c r="D109"/>
+      <c r="E109"/>
+      <c r="F109"/>
+      <c r="G109"/>
+      <c r="H109"/>
+      <c r="I109"/>
+      <c r="J109"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110" s="17"/>
+      <c r="B110"/>
+      <c r="C110"/>
+      <c r="D110"/>
+      <c r="E110"/>
+      <c r="F110"/>
+      <c r="G110"/>
+      <c r="H110"/>
+      <c r="I110"/>
+      <c r="J110"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111" s="17"/>
+      <c r="B111"/>
+      <c r="C111"/>
+      <c r="D111"/>
+      <c r="E111"/>
+      <c r="F111"/>
+      <c r="G111"/>
+      <c r="H111"/>
+      <c r="I111"/>
+      <c r="J111"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112" s="17"/>
+      <c r="B112"/>
+      <c r="C112"/>
+      <c r="D112"/>
+      <c r="E112"/>
+      <c r="F112"/>
+      <c r="G112"/>
+      <c r="H112"/>
+      <c r="I112"/>
+      <c r="J112"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113" s="17"/>
+      <c r="B113"/>
+      <c r="C113"/>
+      <c r="D113"/>
+      <c r="E113"/>
+      <c r="F113"/>
+      <c r="G113"/>
+      <c r="H113"/>
+      <c r="I113"/>
+      <c r="J113"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114" s="17"/>
+      <c r="B114"/>
+      <c r="C114"/>
+      <c r="D114"/>
+      <c r="E114"/>
+      <c r="F114"/>
+      <c r="G114"/>
+      <c r="H114"/>
+      <c r="I114"/>
+      <c r="J114"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" s="17"/>
+      <c r="B115"/>
+      <c r="C115"/>
+      <c r="D115"/>
+      <c r="E115"/>
+      <c r="F115"/>
+      <c r="G115"/>
+      <c r="H115"/>
+      <c r="I115"/>
+      <c r="J115"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" s="17"/>
+      <c r="B116"/>
+      <c r="C116"/>
+      <c r="D116"/>
+      <c r="E116"/>
+      <c r="F116"/>
+      <c r="G116"/>
+      <c r="H116"/>
+      <c r="I116"/>
+      <c r="J116"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117" s="17"/>
+      <c r="B117"/>
+      <c r="C117"/>
+      <c r="D117"/>
+      <c r="E117"/>
+      <c r="F117"/>
+      <c r="G117"/>
+      <c r="H117"/>
+      <c r="I117"/>
+      <c r="J117"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118" s="17"/>
+      <c r="B118"/>
+      <c r="C118"/>
+      <c r="D118"/>
+      <c r="E118"/>
+      <c r="F118"/>
+      <c r="G118"/>
+      <c r="H118"/>
+      <c r="I118"/>
+      <c r="J118"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119" s="17"/>
+      <c r="B119"/>
+      <c r="C119"/>
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="F119"/>
+      <c r="G119"/>
+      <c r="H119"/>
+      <c r="I119"/>
+      <c r="J119"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" s="17"/>
+      <c r="B120"/>
+      <c r="C120"/>
+      <c r="D120"/>
+      <c r="E120"/>
+      <c r="F120"/>
+      <c r="G120"/>
+      <c r="H120"/>
+      <c r="I120"/>
+      <c r="J120"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" s="17"/>
+      <c r="B121"/>
+      <c r="C121"/>
+      <c r="D121"/>
+      <c r="E121"/>
+      <c r="F121"/>
+      <c r="G121"/>
+      <c r="H121"/>
+      <c r="I121"/>
+      <c r="J121"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122" s="17"/>
+      <c r="B122"/>
+      <c r="C122"/>
+      <c r="D122"/>
+      <c r="E122"/>
+      <c r="F122"/>
+      <c r="G122"/>
+      <c r="H122"/>
+      <c r="I122"/>
+      <c r="J122"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" s="17"/>
+      <c r="B123"/>
+      <c r="C123"/>
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123"/>
+      <c r="G123"/>
+      <c r="H123"/>
+      <c r="I123"/>
+      <c r="J123"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" s="17"/>
+      <c r="B124"/>
+      <c r="C124"/>
+      <c r="D124"/>
+      <c r="E124"/>
+      <c r="F124"/>
+      <c r="G124"/>
+      <c r="H124"/>
+      <c r="I124"/>
+      <c r="J124"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" s="17"/>
+      <c r="B125"/>
+      <c r="C125"/>
+      <c r="D125"/>
+      <c r="E125"/>
+      <c r="F125"/>
+      <c r="G125"/>
+      <c r="H125"/>
+      <c r="I125"/>
+      <c r="J125"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" s="17"/>
+      <c r="B126"/>
+      <c r="C126"/>
+      <c r="D126"/>
+      <c r="E126"/>
+      <c r="F126"/>
+      <c r="G126"/>
+      <c r="H126"/>
+      <c r="I126"/>
+      <c r="J126"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A127" s="17"/>
+      <c r="B127"/>
+      <c r="C127"/>
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127"/>
+      <c r="G127"/>
+      <c r="H127"/>
+      <c r="I127"/>
+      <c r="J127"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A128" s="17"/>
+      <c r="B128"/>
+      <c r="C128"/>
+      <c r="D128"/>
+      <c r="E128"/>
+      <c r="F128"/>
+      <c r="G128"/>
+      <c r="H128"/>
+      <c r="I128"/>
+      <c r="J128"/>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A129" s="17"/>
+      <c r="B129"/>
+      <c r="C129"/>
+      <c r="D129"/>
+      <c r="E129"/>
+      <c r="F129"/>
+      <c r="G129"/>
+      <c r="H129"/>
+      <c r="I129"/>
+      <c r="J129"/>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A130" s="17"/>
+      <c r="B130"/>
+      <c r="C130"/>
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130"/>
+      <c r="G130"/>
+      <c r="H130"/>
+      <c r="I130"/>
+      <c r="J130"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A131" s="17"/>
+      <c r="B131"/>
+      <c r="C131"/>
+      <c r="D131"/>
+      <c r="E131"/>
+      <c r="F131"/>
+      <c r="G131"/>
+      <c r="H131"/>
+      <c r="I131"/>
+      <c r="J131"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A132" s="17"/>
+      <c r="B132"/>
+      <c r="C132"/>
+      <c r="D132"/>
+      <c r="E132"/>
+      <c r="F132"/>
+      <c r="G132"/>
+      <c r="H132"/>
+      <c r="I132"/>
+      <c r="J132"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A133" s="17"/>
+      <c r="B133"/>
+      <c r="C133"/>
+      <c r="D133"/>
+      <c r="E133"/>
+      <c r="F133"/>
+      <c r="G133"/>
+      <c r="H133"/>
+      <c r="I133"/>
+      <c r="J133"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A134" s="17"/>
+      <c r="B134"/>
+      <c r="C134"/>
+      <c r="D134"/>
+      <c r="E134"/>
+      <c r="F134"/>
+      <c r="G134"/>
+      <c r="H134"/>
+      <c r="I134"/>
+      <c r="J134"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A135" s="17"/>
+      <c r="B135"/>
+      <c r="C135"/>
+      <c r="D135"/>
+      <c r="E135"/>
+      <c r="F135"/>
+      <c r="G135"/>
+      <c r="H135"/>
+      <c r="I135"/>
+      <c r="J135"/>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A136" s="17"/>
+      <c r="B136"/>
+      <c r="C136"/>
+      <c r="D136"/>
+      <c r="E136"/>
+      <c r="F136"/>
+      <c r="G136"/>
+      <c r="H136"/>
+      <c r="I136"/>
+      <c r="J136"/>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A137" s="17"/>
+      <c r="B137"/>
+      <c r="C137"/>
+      <c r="D137"/>
+      <c r="E137"/>
+      <c r="F137"/>
+      <c r="G137"/>
+      <c r="H137"/>
+      <c r="I137"/>
+      <c r="J137"/>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A138" s="17"/>
+      <c r="B138"/>
+      <c r="C138"/>
+      <c r="D138"/>
+      <c r="E138"/>
+      <c r="F138"/>
+      <c r="G138"/>
+      <c r="H138"/>
+      <c r="I138"/>
+      <c r="J138"/>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A139" s="17"/>
+      <c r="B139"/>
+      <c r="C139"/>
+      <c r="D139"/>
+      <c r="E139"/>
+      <c r="F139"/>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139"/>
+      <c r="J139"/>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A140" s="17"/>
+      <c r="B140"/>
+      <c r="C140"/>
+      <c r="D140"/>
+      <c r="E140"/>
+      <c r="F140"/>
+      <c r="G140"/>
+      <c r="H140"/>
+      <c r="I140"/>
+      <c r="J140"/>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A141" s="17"/>
+      <c r="B141"/>
+      <c r="C141"/>
+      <c r="D141"/>
+      <c r="E141"/>
+      <c r="F141"/>
+      <c r="G141"/>
+      <c r="H141"/>
+      <c r="I141"/>
+      <c r="J141"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -652,7 +2332,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strategy" prompt="Please select strategy from dropdown list" xr:uid="{46A140AA-8190-4C69-86E3-B269F7CB5240}">
           <x14:formula1>
-            <xm:f>ListOfValues!$B$2:$B$3</xm:f>
+            <xm:f>ListOfValues!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
@@ -673,7 +2353,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +2408,9 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C4" s="7" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Fixed bug where we were pulling 200 extra lines when only 50 needed by strategy.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57013416-244D-400A-8DB3-E09F593BDC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4968E6-030C-4B06-B5ED-DBE2204EC589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1536" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,13 +583,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44470</v>
+        <v>44197</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -615,13 +615,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44470</v>
+        <v>44197</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
@@ -639,40 +639,12 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="12">
-        <v>44470</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="16">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>

</xml_diff>

<commit_message>
Updated fees mecanism to pay from account balance.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4968E6-030C-4B06-B5ED-DBE2204EC589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8333E34-BE2F-49C8-8927-A244B15624D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1536" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44197</v>
+        <v>44501</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44197</v>
+        <v>44501</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
@@ -639,12 +639,40 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12">
+        <v>44501</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>

</xml_diff>

<commit_message>
Enter trade with close price instead of open.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8333E34-BE2F-49C8-8927-A244B15624D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F61CAF0-4069-477D-A23A-2C41FAC5455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1536" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -528,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
@@ -615,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -639,40 +639,20 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="12">
-        <v>44501</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="16">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4" s="17"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
@@ -2293,30 +2273,6 @@
       <c r="H139"/>
       <c r="I139"/>
       <c r="J139"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A140" s="17"/>
-      <c r="B140"/>
-      <c r="C140"/>
-      <c r="D140"/>
-      <c r="E140"/>
-      <c r="F140"/>
-      <c r="G140"/>
-      <c r="H140"/>
-      <c r="I140"/>
-      <c r="J140"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A141" s="17"/>
-      <c r="B141"/>
-      <c r="C141"/>
-      <c r="D141"/>
-      <c r="E141"/>
-      <c r="F141"/>
-      <c r="G141"/>
-      <c r="H141"/>
-      <c r="I141"/>
-      <c r="J141"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added RSI_MIN_LIMIT_ENTRY and RSI_MAX_LIMIT_ENTRY settings for Scalping1.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F61CAF0-4069-477D-A23A-2C41FAC5455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1676A9B7-61AC-46B6-B224-1C25EC0BAAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1536" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="2232" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44501</v>
+        <v>44531</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44501</v>
+        <v>44531</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>

</xml_diff>

<commit_message>
Fixed bug in wallet balance on trade entries.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C5ECE4-A05D-4E10-A9CE-2055D251334A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC75F55F-4D31-427B-803A-5216C426F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="696" yWindow="2232" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44531</v>
+        <v>44197</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -615,19 +615,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44531</v>
+        <v>44470</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
@@ -639,20 +639,12 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>

</xml_diff>

<commit_message>
Removed rounding on fees that made balance go negative on Binance.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41BAB5E-DD31-45DF-9448-456B2D8A3651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A84993-2EDE-4F0D-B932-46C04A92C94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="2232" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,10 +601,10 @@
         <v>10000</v>
       </c>
       <c r="H2" s="16">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="I2" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
@@ -633,10 +633,10 @@
         <v>10000</v>
       </c>
       <c r="H3" s="16">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="I3" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Split backtesting in multiple steps common to all strategies.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A84993-2EDE-4F0D-B932-46C04A92C94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1891823-5DE9-484C-9C70-E45A50B19360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,7 +589,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44470</v>
+        <v>44501</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -601,10 +601,10 @@
         <v>10000</v>
       </c>
       <c r="H2" s="16">
-        <v>0.75</v>
+        <v>1.2</v>
       </c>
       <c r="I2" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
@@ -621,30 +621,58 @@
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44470</v>
+        <v>44501</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
       </c>
       <c r="H3" s="16">
-        <v>0.75</v>
+        <v>1.2</v>
       </c>
       <c r="I3" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12">
+        <v>44501</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="16">
+        <v>1.2</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>

</xml_diff>

<commit_message>
Allowed to created Early version of any strategy using multiple inheritance.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1891823-5DE9-484C-9C70-E45A50B19360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325F978B-6B34-4487-B438-E5C7707C0970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,13 +583,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44501</v>
+        <v>44378</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -621,7 +621,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44501</v>
+        <v>44378</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
@@ -639,40 +639,12 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="12">
-        <v>44501</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="I4" s="16">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>

</xml_diff>

<commit_message>
Fixed statistics bug in calculations.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325F978B-6B34-4487-B438-E5C7707C0970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5339B3A-E856-40E2-BCEF-DD7796E2EB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +595,7 @@
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>

</xml_diff>

<commit_message>
Added condition filter in Scalping1 strategy.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5339B3A-E856-40E2-BCEF-DD7796E2EB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD946920-C15B-4BFD-BB4C-72A1C870BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,13 +589,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44378</v>
+        <v>44531</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -621,13 +621,13 @@
         <v>15</v>
       </c>
       <c r="D3" s="12">
-        <v>44378</v>
+        <v>44531</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added timeout handleling for exchange data downloads.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD946920-C15B-4BFD-BB4C-72A1C870BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD22AF9-51CE-402E-8F2E-E850A6A319F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -531,7 +531,7 @@
   <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Fixed trade entry bug in ScalpingEmaRsiAdx strategy.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD22AF9-51CE-402E-8F2E-E850A6A319F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4041A1-B2E6-4168-A3A4-5DD3621405B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -121,7 +121,7 @@
     <t>Initial Capital</t>
   </si>
   <si>
-    <t>Scalping1</t>
+    <t>ScalpingEmaRsiAdx</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,7 +247,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J139"/>
+  <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +542,7 @@
     <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6.88671875" style="16" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -583,75 +582,46 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44531</v>
+        <v>44440</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
       </c>
       <c r="H2" s="16">
-        <v>1.2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I2" s="16">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="12">
-        <v>44531</v>
-      </c>
-      <c r="E3" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="I3" s="16">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5"/>
+      <c r="B5" s="1"/>
       <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
       <c r="F5"/>
       <c r="G5"/>
       <c r="H5"/>
@@ -659,11 +629,10 @@
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6"/>
+      <c r="B6" s="1"/>
       <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
@@ -671,11 +640,10 @@
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7"/>
+      <c r="B7" s="1"/>
       <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7"/>
@@ -683,11 +651,10 @@
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8"/>
+      <c r="B8" s="1"/>
       <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
@@ -695,11 +662,10 @@
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9"/>
+      <c r="B9" s="1"/>
       <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -707,11 +673,10 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10"/>
+      <c r="B10" s="1"/>
       <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10"/>
@@ -719,11 +684,10 @@
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11"/>
+      <c r="B11" s="1"/>
       <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
@@ -731,11 +695,10 @@
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12"/>
+      <c r="B12" s="1"/>
       <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
@@ -743,11 +706,10 @@
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13"/>
+      <c r="B13" s="1"/>
       <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13"/>
@@ -755,11 +717,10 @@
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14"/>
+      <c r="B14" s="1"/>
       <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
@@ -767,11 +728,10 @@
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15"/>
+      <c r="B15" s="1"/>
       <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
@@ -779,1492 +739,1335 @@
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16"/>
+      <c r="B16" s="1"/>
       <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17"/>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
       <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18"/>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
       <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19"/>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
       <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20"/>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
       <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21"/>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
       <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22"/>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
       <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23"/>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
       <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24"/>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
       <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25"/>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
       <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26"/>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
       <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27"/>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
       <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28"/>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
       <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29"/>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
       <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30"/>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
       <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31"/>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
       <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
       <c r="F31"/>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32"/>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
       <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33"/>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
       <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="17"/>
-      <c r="B34"/>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
       <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
       <c r="F34"/>
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="17"/>
-      <c r="B35"/>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
       <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
       <c r="F35"/>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
-      <c r="B36"/>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
       <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
       <c r="F36"/>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
-      <c r="B37"/>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
       <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
       <c r="F37"/>
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="17"/>
-      <c r="B38"/>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
       <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
       <c r="F38"/>
       <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="17"/>
-      <c r="B39"/>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
       <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
       <c r="F39"/>
       <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="17"/>
-      <c r="B40"/>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
       <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
       <c r="F40"/>
       <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41"/>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
       <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42"/>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
       <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="17"/>
-      <c r="B43"/>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
       <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="17"/>
-      <c r="B44"/>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
       <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45"/>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
       <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="17"/>
-      <c r="B46"/>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
       <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
       <c r="F46"/>
       <c r="G46"/>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="17"/>
-      <c r="B47"/>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
       <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
       <c r="F47"/>
       <c r="G47"/>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48"/>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
       <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
       <c r="F48"/>
       <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="17"/>
-      <c r="B49"/>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
       <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
       <c r="F49"/>
       <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50"/>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
       <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
       <c r="F50"/>
       <c r="G50"/>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
-      <c r="B51"/>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
       <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
       <c r="F51"/>
       <c r="G51"/>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="17"/>
-      <c r="B52"/>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
       <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
       <c r="F52"/>
       <c r="G52"/>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="17"/>
-      <c r="B53"/>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
       <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
       <c r="F53"/>
       <c r="G53"/>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
-      <c r="B54"/>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
       <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
       <c r="F54"/>
       <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="17"/>
-      <c r="B55"/>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
       <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
       <c r="F55"/>
       <c r="G55"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56"/>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
       <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
       <c r="F56"/>
       <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="17"/>
-      <c r="B57"/>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
       <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
       <c r="F57"/>
       <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58"/>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
       <c r="C58"/>
-      <c r="D58"/>
-      <c r="E58"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
       <c r="F58"/>
       <c r="G58"/>
       <c r="H58"/>
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59"/>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
       <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
       <c r="F59"/>
       <c r="G59"/>
       <c r="H59"/>
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60"/>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
       <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
       <c r="F60"/>
       <c r="G60"/>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="17"/>
-      <c r="B61"/>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
       <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
       <c r="F61"/>
       <c r="G61"/>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62"/>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
       <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
       <c r="F62"/>
       <c r="G62"/>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63"/>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
       <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
       <c r="F63"/>
       <c r="G63"/>
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="17"/>
-      <c r="B64"/>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
       <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
       <c r="F64"/>
       <c r="G64"/>
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="17"/>
-      <c r="B65"/>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
       <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
       <c r="F65"/>
       <c r="G65"/>
       <c r="H65"/>
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66"/>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
       <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
       <c r="F66"/>
       <c r="G66"/>
       <c r="H66"/>
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="17"/>
-      <c r="B67"/>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
       <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
       <c r="F67"/>
       <c r="G67"/>
       <c r="H67"/>
       <c r="I67"/>
       <c r="J67"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="17"/>
-      <c r="B68"/>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
       <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
       <c r="F68"/>
       <c r="G68"/>
       <c r="H68"/>
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" s="17"/>
-      <c r="B69"/>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
       <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
       <c r="F69"/>
       <c r="G69"/>
       <c r="H69"/>
       <c r="I69"/>
       <c r="J69"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70"/>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
       <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
       <c r="F70"/>
       <c r="G70"/>
       <c r="H70"/>
       <c r="I70"/>
       <c r="J70"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="17"/>
-      <c r="B71"/>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
       <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
       <c r="F71"/>
       <c r="G71"/>
       <c r="H71"/>
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72"/>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
       <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
       <c r="F72"/>
       <c r="G72"/>
       <c r="H72"/>
       <c r="I72"/>
       <c r="J72"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A73" s="17"/>
-      <c r="B73"/>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
       <c r="C73"/>
-      <c r="D73"/>
-      <c r="E73"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
       <c r="F73"/>
       <c r="G73"/>
       <c r="H73"/>
       <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74"/>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
       <c r="C74"/>
-      <c r="D74"/>
-      <c r="E74"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
       <c r="F74"/>
       <c r="G74"/>
       <c r="H74"/>
       <c r="I74"/>
       <c r="J74"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="17"/>
-      <c r="B75"/>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
       <c r="C75"/>
-      <c r="D75"/>
-      <c r="E75"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
       <c r="F75"/>
       <c r="G75"/>
       <c r="H75"/>
       <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="17"/>
-      <c r="B76"/>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
       <c r="C76"/>
-      <c r="D76"/>
-      <c r="E76"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
       <c r="F76"/>
       <c r="G76"/>
       <c r="H76"/>
       <c r="I76"/>
       <c r="J76"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="17"/>
-      <c r="B77"/>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
       <c r="C77"/>
-      <c r="D77"/>
-      <c r="E77"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
       <c r="F77"/>
       <c r="G77"/>
       <c r="H77"/>
       <c r="I77"/>
       <c r="J77"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="17"/>
-      <c r="B78"/>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
       <c r="C78"/>
-      <c r="D78"/>
-      <c r="E78"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
       <c r="F78"/>
       <c r="G78"/>
       <c r="H78"/>
       <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="17"/>
-      <c r="B79"/>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
       <c r="C79"/>
-      <c r="D79"/>
-      <c r="E79"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
       <c r="F79"/>
       <c r="G79"/>
       <c r="H79"/>
       <c r="I79"/>
       <c r="J79"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A80" s="17"/>
-      <c r="B80"/>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
       <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
       <c r="F80"/>
       <c r="G80"/>
       <c r="H80"/>
       <c r="I80"/>
       <c r="J80"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A81" s="17"/>
-      <c r="B81"/>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
       <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
       <c r="F81"/>
       <c r="G81"/>
       <c r="H81"/>
       <c r="I81"/>
       <c r="J81"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="17"/>
-      <c r="B82"/>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
       <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
       <c r="F82"/>
       <c r="G82"/>
       <c r="H82"/>
       <c r="I82"/>
       <c r="J82"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="17"/>
-      <c r="B83"/>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
       <c r="C83"/>
-      <c r="D83"/>
-      <c r="E83"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
       <c r="F83"/>
       <c r="G83"/>
       <c r="H83"/>
       <c r="I83"/>
       <c r="J83"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="17"/>
-      <c r="B84"/>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B84" s="1"/>
       <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
       <c r="F84"/>
       <c r="G84"/>
       <c r="H84"/>
       <c r="I84"/>
       <c r="J84"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="17"/>
-      <c r="B85"/>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
       <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
       <c r="F85"/>
       <c r="G85"/>
       <c r="H85"/>
       <c r="I85"/>
       <c r="J85"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="17"/>
-      <c r="B86"/>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
       <c r="C86"/>
-      <c r="D86"/>
-      <c r="E86"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
       <c r="F86"/>
       <c r="G86"/>
       <c r="H86"/>
       <c r="I86"/>
       <c r="J86"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="17"/>
-      <c r="B87"/>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
       <c r="C87"/>
-      <c r="D87"/>
-      <c r="E87"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
       <c r="F87"/>
       <c r="G87"/>
       <c r="H87"/>
       <c r="I87"/>
       <c r="J87"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A88" s="17"/>
-      <c r="B88"/>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
       <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
       <c r="F88"/>
       <c r="G88"/>
       <c r="H88"/>
       <c r="I88"/>
       <c r="J88"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A89" s="17"/>
-      <c r="B89"/>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
       <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
       <c r="F89"/>
       <c r="G89"/>
       <c r="H89"/>
       <c r="I89"/>
       <c r="J89"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="17"/>
-      <c r="B90"/>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
       <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
       <c r="F90"/>
       <c r="G90"/>
       <c r="H90"/>
       <c r="I90"/>
       <c r="J90"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="17"/>
-      <c r="B91"/>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
       <c r="C91"/>
-      <c r="D91"/>
-      <c r="E91"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
       <c r="F91"/>
       <c r="G91"/>
       <c r="H91"/>
       <c r="I91"/>
       <c r="J91"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="17"/>
-      <c r="B92"/>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
       <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
       <c r="F92"/>
       <c r="G92"/>
       <c r="H92"/>
       <c r="I92"/>
       <c r="J92"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="17"/>
-      <c r="B93"/>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
       <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
       <c r="F93"/>
       <c r="G93"/>
       <c r="H93"/>
       <c r="I93"/>
       <c r="J93"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94" s="17"/>
-      <c r="B94"/>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
       <c r="C94"/>
-      <c r="D94"/>
-      <c r="E94"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
       <c r="F94"/>
       <c r="G94"/>
       <c r="H94"/>
       <c r="I94"/>
       <c r="J94"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A95" s="17"/>
-      <c r="B95"/>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
       <c r="C95"/>
-      <c r="D95"/>
-      <c r="E95"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
       <c r="F95"/>
       <c r="G95"/>
       <c r="H95"/>
       <c r="I95"/>
       <c r="J95"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="17"/>
-      <c r="B96"/>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
       <c r="C96"/>
-      <c r="D96"/>
-      <c r="E96"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
       <c r="F96"/>
       <c r="G96"/>
       <c r="H96"/>
       <c r="I96"/>
       <c r="J96"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A97" s="17"/>
-      <c r="B97"/>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
       <c r="C97"/>
-      <c r="D97"/>
-      <c r="E97"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
       <c r="F97"/>
       <c r="G97"/>
       <c r="H97"/>
       <c r="I97"/>
       <c r="J97"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A98" s="17"/>
-      <c r="B98"/>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
       <c r="C98"/>
-      <c r="D98"/>
-      <c r="E98"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
       <c r="F98"/>
       <c r="G98"/>
       <c r="H98"/>
       <c r="I98"/>
       <c r="J98"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A99" s="17"/>
-      <c r="B99"/>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
       <c r="C99"/>
-      <c r="D99"/>
-      <c r="E99"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
       <c r="F99"/>
       <c r="G99"/>
       <c r="H99"/>
       <c r="I99"/>
       <c r="J99"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A100" s="17"/>
-      <c r="B100"/>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
       <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
       <c r="F100"/>
       <c r="G100"/>
       <c r="H100"/>
       <c r="I100"/>
       <c r="J100"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A101" s="17"/>
-      <c r="B101"/>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
       <c r="C101"/>
-      <c r="D101"/>
-      <c r="E101"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
       <c r="F101"/>
       <c r="G101"/>
       <c r="H101"/>
       <c r="I101"/>
       <c r="J101"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A102" s="17"/>
-      <c r="B102"/>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
       <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
       <c r="F102"/>
       <c r="G102"/>
       <c r="H102"/>
       <c r="I102"/>
       <c r="J102"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A103" s="17"/>
-      <c r="B103"/>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
       <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
       <c r="F103"/>
       <c r="G103"/>
       <c r="H103"/>
       <c r="I103"/>
       <c r="J103"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A104" s="17"/>
-      <c r="B104"/>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B104" s="1"/>
       <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
       <c r="F104"/>
       <c r="G104"/>
       <c r="H104"/>
       <c r="I104"/>
       <c r="J104"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A105" s="17"/>
-      <c r="B105"/>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B105" s="1"/>
       <c r="C105"/>
-      <c r="D105"/>
-      <c r="E105"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
       <c r="F105"/>
       <c r="G105"/>
       <c r="H105"/>
       <c r="I105"/>
       <c r="J105"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A106" s="17"/>
-      <c r="B106"/>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B106" s="1"/>
       <c r="C106"/>
-      <c r="D106"/>
-      <c r="E106"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
       <c r="F106"/>
       <c r="G106"/>
       <c r="H106"/>
       <c r="I106"/>
       <c r="J106"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A107" s="17"/>
-      <c r="B107"/>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B107" s="1"/>
       <c r="C107"/>
-      <c r="D107"/>
-      <c r="E107"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
       <c r="F107"/>
       <c r="G107"/>
       <c r="H107"/>
       <c r="I107"/>
       <c r="J107"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A108" s="17"/>
-      <c r="B108"/>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
       <c r="C108"/>
-      <c r="D108"/>
-      <c r="E108"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
       <c r="F108"/>
       <c r="G108"/>
       <c r="H108"/>
       <c r="I108"/>
       <c r="J108"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A109" s="17"/>
-      <c r="B109"/>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B109" s="1"/>
       <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
       <c r="F109"/>
       <c r="G109"/>
       <c r="H109"/>
       <c r="I109"/>
       <c r="J109"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A110" s="17"/>
-      <c r="B110"/>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B110" s="1"/>
       <c r="C110"/>
-      <c r="D110"/>
-      <c r="E110"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
       <c r="F110"/>
       <c r="G110"/>
       <c r="H110"/>
       <c r="I110"/>
       <c r="J110"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A111" s="17"/>
-      <c r="B111"/>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B111" s="1"/>
       <c r="C111"/>
-      <c r="D111"/>
-      <c r="E111"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
       <c r="F111"/>
       <c r="G111"/>
       <c r="H111"/>
       <c r="I111"/>
       <c r="J111"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A112" s="17"/>
-      <c r="B112"/>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B112" s="1"/>
       <c r="C112"/>
-      <c r="D112"/>
-      <c r="E112"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
       <c r="F112"/>
       <c r="G112"/>
       <c r="H112"/>
       <c r="I112"/>
       <c r="J112"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A113" s="17"/>
-      <c r="B113"/>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B113" s="1"/>
       <c r="C113"/>
-      <c r="D113"/>
-      <c r="E113"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
       <c r="F113"/>
       <c r="G113"/>
       <c r="H113"/>
       <c r="I113"/>
       <c r="J113"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A114" s="17"/>
-      <c r="B114"/>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B114" s="1"/>
       <c r="C114"/>
-      <c r="D114"/>
-      <c r="E114"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
       <c r="F114"/>
       <c r="G114"/>
       <c r="H114"/>
       <c r="I114"/>
       <c r="J114"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A115" s="17"/>
-      <c r="B115"/>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B115" s="1"/>
       <c r="C115"/>
-      <c r="D115"/>
-      <c r="E115"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
       <c r="F115"/>
       <c r="G115"/>
       <c r="H115"/>
       <c r="I115"/>
       <c r="J115"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A116" s="17"/>
-      <c r="B116"/>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B116" s="1"/>
       <c r="C116"/>
-      <c r="D116"/>
-      <c r="E116"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
       <c r="F116"/>
       <c r="G116"/>
       <c r="H116"/>
       <c r="I116"/>
       <c r="J116"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A117" s="17"/>
-      <c r="B117"/>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B117" s="1"/>
       <c r="C117"/>
-      <c r="D117"/>
-      <c r="E117"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
       <c r="F117"/>
       <c r="G117"/>
       <c r="H117"/>
       <c r="I117"/>
       <c r="J117"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A118" s="17"/>
-      <c r="B118"/>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B118" s="1"/>
       <c r="C118"/>
-      <c r="D118"/>
-      <c r="E118"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
       <c r="F118"/>
       <c r="G118"/>
       <c r="H118"/>
       <c r="I118"/>
       <c r="J118"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A119" s="17"/>
-      <c r="B119"/>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B119" s="1"/>
       <c r="C119"/>
-      <c r="D119"/>
-      <c r="E119"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
       <c r="F119"/>
       <c r="G119"/>
       <c r="H119"/>
       <c r="I119"/>
       <c r="J119"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A120" s="17"/>
-      <c r="B120"/>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B120" s="1"/>
       <c r="C120"/>
-      <c r="D120"/>
-      <c r="E120"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
       <c r="F120"/>
       <c r="G120"/>
       <c r="H120"/>
       <c r="I120"/>
       <c r="J120"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A121" s="17"/>
-      <c r="B121"/>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B121" s="1"/>
       <c r="C121"/>
-      <c r="D121"/>
-      <c r="E121"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
       <c r="F121"/>
       <c r="G121"/>
       <c r="H121"/>
       <c r="I121"/>
       <c r="J121"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A122" s="17"/>
-      <c r="B122"/>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B122" s="1"/>
       <c r="C122"/>
-      <c r="D122"/>
-      <c r="E122"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
       <c r="F122"/>
       <c r="G122"/>
       <c r="H122"/>
       <c r="I122"/>
       <c r="J122"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A123" s="17"/>
-      <c r="B123"/>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B123" s="1"/>
       <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
       <c r="F123"/>
       <c r="G123"/>
       <c r="H123"/>
       <c r="I123"/>
       <c r="J123"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A124" s="17"/>
-      <c r="B124"/>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B124" s="1"/>
       <c r="C124"/>
-      <c r="D124"/>
-      <c r="E124"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
       <c r="F124"/>
       <c r="G124"/>
       <c r="H124"/>
       <c r="I124"/>
       <c r="J124"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A125" s="17"/>
-      <c r="B125"/>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B125" s="1"/>
       <c r="C125"/>
-      <c r="D125"/>
-      <c r="E125"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
       <c r="F125"/>
       <c r="G125"/>
       <c r="H125"/>
       <c r="I125"/>
       <c r="J125"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A126" s="17"/>
-      <c r="B126"/>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B126" s="1"/>
       <c r="C126"/>
-      <c r="D126"/>
-      <c r="E126"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
       <c r="F126"/>
       <c r="G126"/>
       <c r="H126"/>
       <c r="I126"/>
       <c r="J126"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A127" s="17"/>
-      <c r="B127"/>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B127" s="1"/>
       <c r="C127"/>
-      <c r="D127"/>
-      <c r="E127"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
       <c r="F127"/>
       <c r="G127"/>
       <c r="H127"/>
       <c r="I127"/>
       <c r="J127"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A128" s="17"/>
-      <c r="B128"/>
+    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B128" s="1"/>
       <c r="C128"/>
-      <c r="D128"/>
-      <c r="E128"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
       <c r="F128"/>
       <c r="G128"/>
       <c r="H128"/>
       <c r="I128"/>
       <c r="J128"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A129" s="17"/>
-      <c r="B129"/>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B129" s="1"/>
       <c r="C129"/>
-      <c r="D129"/>
-      <c r="E129"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
       <c r="F129"/>
       <c r="G129"/>
       <c r="H129"/>
       <c r="I129"/>
       <c r="J129"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A130" s="17"/>
-      <c r="B130"/>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B130" s="1"/>
       <c r="C130"/>
-      <c r="D130"/>
-      <c r="E130"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
       <c r="F130"/>
       <c r="G130"/>
       <c r="H130"/>
       <c r="I130"/>
       <c r="J130"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A131" s="17"/>
-      <c r="B131"/>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B131" s="1"/>
       <c r="C131"/>
-      <c r="D131"/>
-      <c r="E131"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
       <c r="F131"/>
       <c r="G131"/>
       <c r="H131"/>
       <c r="I131"/>
       <c r="J131"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A132" s="17"/>
-      <c r="B132"/>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B132" s="1"/>
       <c r="C132"/>
-      <c r="D132"/>
-      <c r="E132"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
       <c r="F132"/>
       <c r="G132"/>
       <c r="H132"/>
       <c r="I132"/>
       <c r="J132"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A133" s="17"/>
-      <c r="B133"/>
+    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B133" s="1"/>
       <c r="C133"/>
-      <c r="D133"/>
-      <c r="E133"/>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
       <c r="F133"/>
       <c r="G133"/>
       <c r="H133"/>
       <c r="I133"/>
       <c r="J133"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A134" s="17"/>
-      <c r="B134"/>
+    <row r="134" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B134" s="1"/>
       <c r="C134"/>
-      <c r="D134"/>
-      <c r="E134"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
       <c r="F134"/>
       <c r="G134"/>
       <c r="H134"/>
       <c r="I134"/>
       <c r="J134"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A135" s="17"/>
-      <c r="B135"/>
+    <row r="135" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B135" s="1"/>
       <c r="C135"/>
-      <c r="D135"/>
-      <c r="E135"/>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
       <c r="F135"/>
       <c r="G135"/>
       <c r="H135"/>
       <c r="I135"/>
       <c r="J135"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A136" s="17"/>
-      <c r="B136"/>
+    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B136" s="1"/>
       <c r="C136"/>
-      <c r="D136"/>
-      <c r="E136"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
       <c r="F136"/>
       <c r="G136"/>
       <c r="H136"/>
       <c r="I136"/>
       <c r="J136"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A137" s="17"/>
-      <c r="B137"/>
-      <c r="C137"/>
-      <c r="D137"/>
-      <c r="E137"/>
-      <c r="F137"/>
-      <c r="G137"/>
-      <c r="H137"/>
-      <c r="I137"/>
-      <c r="J137"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A138" s="17"/>
-      <c r="B138"/>
-      <c r="C138"/>
-      <c r="D138"/>
-      <c r="E138"/>
-      <c r="F138"/>
-      <c r="G138"/>
-      <c r="H138"/>
-      <c r="I138"/>
-      <c r="J138"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A139" s="17"/>
-      <c r="B139"/>
-      <c r="C139"/>
-      <c r="D139"/>
-      <c r="E139"/>
-      <c r="F139"/>
-      <c r="G139"/>
-      <c r="H139"/>
-      <c r="I139"/>
-      <c r="J139"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2301,13 +2104,13 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
     <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Added ByBit2 using ccxt library.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4041A1-B2E6-4168-A3A4-5DD3621405B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1554B86-3CCA-4DB4-82F5-B6498BFCC552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1548" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Interval</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>ScalpingEmaRsiAdx</t>
+  </si>
+  <si>
+    <t>ByBit2</t>
   </si>
 </sst>
 </file>
@@ -199,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,12 +243,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,7 +527,7 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +538,7 @@
     <col min="4" max="5" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.88671875" style="16" customWidth="1"/>
+    <col min="8" max="9" width="6.88671875" style="8" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -567,10 +564,10 @@
       <c r="G1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -582,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
@@ -594,19 +591,19 @@
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="8">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="8">
         <v>2.2999999999999998</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -618,26 +615,12 @@
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
@@ -646,8 +629,6 @@
       <c r="E7" s="12"/>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
       <c r="J7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -657,8 +638,6 @@
       <c r="E8" s="12"/>
       <c r="F8"/>
       <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
       <c r="J8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -668,8 +647,6 @@
       <c r="E9" s="12"/>
       <c r="F9"/>
       <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -679,8 +656,6 @@
       <c r="E10" s="12"/>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -690,8 +665,6 @@
       <c r="E11" s="12"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -701,8 +674,6 @@
       <c r="E12" s="12"/>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -712,8 +683,6 @@
       <c r="E13" s="12"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -723,8 +692,6 @@
       <c r="E14" s="12"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -734,8 +701,6 @@
       <c r="E15" s="12"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -745,8 +710,6 @@
       <c r="E16" s="12"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
       <c r="J16"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
@@ -756,8 +719,6 @@
       <c r="E17" s="12"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
       <c r="J17"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
@@ -767,8 +728,6 @@
       <c r="E18" s="12"/>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
       <c r="J18"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
@@ -778,8 +737,6 @@
       <c r="E19" s="12"/>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
@@ -789,8 +746,6 @@
       <c r="E20" s="12"/>
       <c r="F20"/>
       <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
       <c r="J20"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
@@ -800,8 +755,6 @@
       <c r="E21" s="12"/>
       <c r="F21"/>
       <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
       <c r="J21"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
@@ -811,8 +764,6 @@
       <c r="E22" s="12"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
       <c r="J22"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
@@ -822,8 +773,6 @@
       <c r="E23" s="12"/>
       <c r="F23"/>
       <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
@@ -833,8 +782,6 @@
       <c r="E24" s="12"/>
       <c r="F24"/>
       <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
       <c r="J24"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
@@ -844,8 +791,6 @@
       <c r="E25" s="12"/>
       <c r="F25"/>
       <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
       <c r="J25"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
@@ -855,8 +800,6 @@
       <c r="E26" s="12"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
       <c r="J26"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
@@ -866,8 +809,6 @@
       <c r="E27" s="12"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
       <c r="J27"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
@@ -877,8 +818,6 @@
       <c r="E28" s="12"/>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
       <c r="J28"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
@@ -888,8 +827,6 @@
       <c r="E29" s="12"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
       <c r="J29"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
@@ -899,8 +836,6 @@
       <c r="E30" s="12"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
       <c r="J30"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
@@ -910,8 +845,6 @@
       <c r="E31" s="12"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
       <c r="J31"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
@@ -921,8 +854,6 @@
       <c r="E32" s="12"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
       <c r="J32"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
@@ -932,8 +863,6 @@
       <c r="E33" s="12"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
       <c r="J33"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
@@ -943,8 +872,6 @@
       <c r="E34" s="12"/>
       <c r="F34"/>
       <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
       <c r="J34"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
@@ -954,8 +881,6 @@
       <c r="E35" s="12"/>
       <c r="F35"/>
       <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
       <c r="J35"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
@@ -965,8 +890,6 @@
       <c r="E36" s="12"/>
       <c r="F36"/>
       <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
       <c r="J36"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
@@ -976,8 +899,6 @@
       <c r="E37" s="12"/>
       <c r="F37"/>
       <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
       <c r="J37"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
@@ -987,8 +908,6 @@
       <c r="E38" s="12"/>
       <c r="F38"/>
       <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
       <c r="J38"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
@@ -998,8 +917,6 @@
       <c r="E39" s="12"/>
       <c r="F39"/>
       <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
       <c r="J39"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
@@ -1009,8 +926,6 @@
       <c r="E40" s="12"/>
       <c r="F40"/>
       <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
       <c r="J40"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
@@ -1020,8 +935,6 @@
       <c r="E41" s="12"/>
       <c r="F41"/>
       <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
       <c r="J41"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
@@ -1031,8 +944,6 @@
       <c r="E42" s="12"/>
       <c r="F42"/>
       <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
       <c r="J42"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
@@ -1042,8 +953,6 @@
       <c r="E43" s="12"/>
       <c r="F43"/>
       <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
       <c r="J43"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
@@ -1053,8 +962,6 @@
       <c r="E44" s="12"/>
       <c r="F44"/>
       <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
       <c r="J44"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
@@ -1064,8 +971,6 @@
       <c r="E45" s="12"/>
       <c r="F45"/>
       <c r="G45"/>
-      <c r="H45"/>
-      <c r="I45"/>
       <c r="J45"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
@@ -1075,8 +980,6 @@
       <c r="E46" s="12"/>
       <c r="F46"/>
       <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
       <c r="J46"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
@@ -1086,8 +989,6 @@
       <c r="E47" s="12"/>
       <c r="F47"/>
       <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
       <c r="J47"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
@@ -1097,8 +998,6 @@
       <c r="E48" s="12"/>
       <c r="F48"/>
       <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
       <c r="J48"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
@@ -1108,8 +1007,6 @@
       <c r="E49" s="12"/>
       <c r="F49"/>
       <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
       <c r="J49"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
@@ -1119,8 +1016,6 @@
       <c r="E50" s="12"/>
       <c r="F50"/>
       <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
       <c r="J50"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
@@ -1130,8 +1025,6 @@
       <c r="E51" s="12"/>
       <c r="F51"/>
       <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
       <c r="J51"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
@@ -1141,8 +1034,6 @@
       <c r="E52" s="12"/>
       <c r="F52"/>
       <c r="G52"/>
-      <c r="H52"/>
-      <c r="I52"/>
       <c r="J52"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
@@ -1152,8 +1043,6 @@
       <c r="E53" s="12"/>
       <c r="F53"/>
       <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
       <c r="J53"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
@@ -1163,8 +1052,6 @@
       <c r="E54" s="12"/>
       <c r="F54"/>
       <c r="G54"/>
-      <c r="H54"/>
-      <c r="I54"/>
       <c r="J54"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
@@ -1174,8 +1061,6 @@
       <c r="E55" s="12"/>
       <c r="F55"/>
       <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
       <c r="J55"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
@@ -1185,8 +1070,6 @@
       <c r="E56" s="12"/>
       <c r="F56"/>
       <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
       <c r="J56"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
@@ -1196,8 +1079,6 @@
       <c r="E57" s="12"/>
       <c r="F57"/>
       <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
       <c r="J57"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
@@ -1207,8 +1088,6 @@
       <c r="E58" s="12"/>
       <c r="F58"/>
       <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
       <c r="J58"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
@@ -1218,8 +1097,6 @@
       <c r="E59" s="12"/>
       <c r="F59"/>
       <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
       <c r="J59"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
@@ -1229,8 +1106,6 @@
       <c r="E60" s="12"/>
       <c r="F60"/>
       <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
       <c r="J60"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
@@ -1240,8 +1115,6 @@
       <c r="E61" s="12"/>
       <c r="F61"/>
       <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
       <c r="J61"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.3">
@@ -1251,8 +1124,6 @@
       <c r="E62" s="12"/>
       <c r="F62"/>
       <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
       <c r="J62"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.3">
@@ -1262,8 +1133,6 @@
       <c r="E63" s="12"/>
       <c r="F63"/>
       <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
       <c r="J63"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
@@ -1273,8 +1142,6 @@
       <c r="E64" s="12"/>
       <c r="F64"/>
       <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
       <c r="J64"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.3">
@@ -1284,8 +1151,6 @@
       <c r="E65" s="12"/>
       <c r="F65"/>
       <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
       <c r="J65"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.3">
@@ -1295,8 +1160,6 @@
       <c r="E66" s="12"/>
       <c r="F66"/>
       <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
       <c r="J66"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.3">
@@ -1306,8 +1169,6 @@
       <c r="E67" s="12"/>
       <c r="F67"/>
       <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
       <c r="J67"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.3">
@@ -1317,8 +1178,6 @@
       <c r="E68" s="12"/>
       <c r="F68"/>
       <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
       <c r="J68"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.3">
@@ -1328,8 +1187,6 @@
       <c r="E69" s="12"/>
       <c r="F69"/>
       <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
       <c r="J69"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.3">
@@ -1339,8 +1196,6 @@
       <c r="E70" s="12"/>
       <c r="F70"/>
       <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
       <c r="J70"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.3">
@@ -1350,8 +1205,6 @@
       <c r="E71" s="12"/>
       <c r="F71"/>
       <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
       <c r="J71"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.3">
@@ -1361,8 +1214,6 @@
       <c r="E72" s="12"/>
       <c r="F72"/>
       <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
       <c r="J72"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.3">
@@ -1372,8 +1223,6 @@
       <c r="E73" s="12"/>
       <c r="F73"/>
       <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
       <c r="J73"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.3">
@@ -1383,8 +1232,6 @@
       <c r="E74" s="12"/>
       <c r="F74"/>
       <c r="G74"/>
-      <c r="H74"/>
-      <c r="I74"/>
       <c r="J74"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.3">
@@ -1394,8 +1241,6 @@
       <c r="E75" s="12"/>
       <c r="F75"/>
       <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
       <c r="J75"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.3">
@@ -1405,8 +1250,6 @@
       <c r="E76" s="12"/>
       <c r="F76"/>
       <c r="G76"/>
-      <c r="H76"/>
-      <c r="I76"/>
       <c r="J76"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.3">
@@ -1416,8 +1259,6 @@
       <c r="E77" s="12"/>
       <c r="F77"/>
       <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
       <c r="J77"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.3">
@@ -1427,8 +1268,6 @@
       <c r="E78" s="12"/>
       <c r="F78"/>
       <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
       <c r="J78"/>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.3">
@@ -1438,8 +1277,6 @@
       <c r="E79" s="12"/>
       <c r="F79"/>
       <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
       <c r="J79"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.3">
@@ -1449,8 +1286,6 @@
       <c r="E80" s="12"/>
       <c r="F80"/>
       <c r="G80"/>
-      <c r="H80"/>
-      <c r="I80"/>
       <c r="J80"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.3">
@@ -1460,8 +1295,6 @@
       <c r="E81" s="12"/>
       <c r="F81"/>
       <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
       <c r="J81"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.3">
@@ -1471,8 +1304,6 @@
       <c r="E82" s="12"/>
       <c r="F82"/>
       <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
       <c r="J82"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.3">
@@ -1482,8 +1313,6 @@
       <c r="E83" s="12"/>
       <c r="F83"/>
       <c r="G83"/>
-      <c r="H83"/>
-      <c r="I83"/>
       <c r="J83"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.3">
@@ -1493,8 +1322,6 @@
       <c r="E84" s="12"/>
       <c r="F84"/>
       <c r="G84"/>
-      <c r="H84"/>
-      <c r="I84"/>
       <c r="J84"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.3">
@@ -1504,8 +1331,6 @@
       <c r="E85" s="12"/>
       <c r="F85"/>
       <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
       <c r="J85"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.3">
@@ -1515,8 +1340,6 @@
       <c r="E86" s="12"/>
       <c r="F86"/>
       <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
       <c r="J86"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.3">
@@ -1526,8 +1349,6 @@
       <c r="E87" s="12"/>
       <c r="F87"/>
       <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
       <c r="J87"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.3">
@@ -1537,8 +1358,6 @@
       <c r="E88" s="12"/>
       <c r="F88"/>
       <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
       <c r="J88"/>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.3">
@@ -1548,8 +1367,6 @@
       <c r="E89" s="12"/>
       <c r="F89"/>
       <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
       <c r="J89"/>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.3">
@@ -1559,8 +1376,6 @@
       <c r="E90" s="12"/>
       <c r="F90"/>
       <c r="G90"/>
-      <c r="H90"/>
-      <c r="I90"/>
       <c r="J90"/>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.3">
@@ -1570,8 +1385,6 @@
       <c r="E91" s="12"/>
       <c r="F91"/>
       <c r="G91"/>
-      <c r="H91"/>
-      <c r="I91"/>
       <c r="J91"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.3">
@@ -1581,8 +1394,6 @@
       <c r="E92" s="12"/>
       <c r="F92"/>
       <c r="G92"/>
-      <c r="H92"/>
-      <c r="I92"/>
       <c r="J92"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.3">
@@ -1592,8 +1403,6 @@
       <c r="E93" s="12"/>
       <c r="F93"/>
       <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
       <c r="J93"/>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.3">
@@ -1603,8 +1412,6 @@
       <c r="E94" s="12"/>
       <c r="F94"/>
       <c r="G94"/>
-      <c r="H94"/>
-      <c r="I94"/>
       <c r="J94"/>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.3">
@@ -1614,8 +1421,6 @@
       <c r="E95" s="12"/>
       <c r="F95"/>
       <c r="G95"/>
-      <c r="H95"/>
-      <c r="I95"/>
       <c r="J95"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.3">
@@ -1625,8 +1430,6 @@
       <c r="E96" s="12"/>
       <c r="F96"/>
       <c r="G96"/>
-      <c r="H96"/>
-      <c r="I96"/>
       <c r="J96"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.3">
@@ -1636,8 +1439,6 @@
       <c r="E97" s="12"/>
       <c r="F97"/>
       <c r="G97"/>
-      <c r="H97"/>
-      <c r="I97"/>
       <c r="J97"/>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.3">
@@ -1647,8 +1448,6 @@
       <c r="E98" s="12"/>
       <c r="F98"/>
       <c r="G98"/>
-      <c r="H98"/>
-      <c r="I98"/>
       <c r="J98"/>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.3">
@@ -1658,8 +1457,6 @@
       <c r="E99" s="12"/>
       <c r="F99"/>
       <c r="G99"/>
-      <c r="H99"/>
-      <c r="I99"/>
       <c r="J99"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.3">
@@ -1669,8 +1466,6 @@
       <c r="E100" s="12"/>
       <c r="F100"/>
       <c r="G100"/>
-      <c r="H100"/>
-      <c r="I100"/>
       <c r="J100"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.3">
@@ -1680,8 +1475,6 @@
       <c r="E101" s="12"/>
       <c r="F101"/>
       <c r="G101"/>
-      <c r="H101"/>
-      <c r="I101"/>
       <c r="J101"/>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.3">
@@ -1691,8 +1484,6 @@
       <c r="E102" s="12"/>
       <c r="F102"/>
       <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
       <c r="J102"/>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.3">
@@ -1702,8 +1493,6 @@
       <c r="E103" s="12"/>
       <c r="F103"/>
       <c r="G103"/>
-      <c r="H103"/>
-      <c r="I103"/>
       <c r="J103"/>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.3">
@@ -1713,8 +1502,6 @@
       <c r="E104" s="12"/>
       <c r="F104"/>
       <c r="G104"/>
-      <c r="H104"/>
-      <c r="I104"/>
       <c r="J104"/>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.3">
@@ -1724,8 +1511,6 @@
       <c r="E105" s="12"/>
       <c r="F105"/>
       <c r="G105"/>
-      <c r="H105"/>
-      <c r="I105"/>
       <c r="J105"/>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.3">
@@ -1735,8 +1520,6 @@
       <c r="E106" s="12"/>
       <c r="F106"/>
       <c r="G106"/>
-      <c r="H106"/>
-      <c r="I106"/>
       <c r="J106"/>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.3">
@@ -1746,8 +1529,6 @@
       <c r="E107" s="12"/>
       <c r="F107"/>
       <c r="G107"/>
-      <c r="H107"/>
-      <c r="I107"/>
       <c r="J107"/>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.3">
@@ -1757,8 +1538,6 @@
       <c r="E108" s="12"/>
       <c r="F108"/>
       <c r="G108"/>
-      <c r="H108"/>
-      <c r="I108"/>
       <c r="J108"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.3">
@@ -1768,8 +1547,6 @@
       <c r="E109" s="12"/>
       <c r="F109"/>
       <c r="G109"/>
-      <c r="H109"/>
-      <c r="I109"/>
       <c r="J109"/>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.3">
@@ -1779,8 +1556,6 @@
       <c r="E110" s="12"/>
       <c r="F110"/>
       <c r="G110"/>
-      <c r="H110"/>
-      <c r="I110"/>
       <c r="J110"/>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.3">
@@ -1790,8 +1565,6 @@
       <c r="E111" s="12"/>
       <c r="F111"/>
       <c r="G111"/>
-      <c r="H111"/>
-      <c r="I111"/>
       <c r="J111"/>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.3">
@@ -1801,8 +1574,6 @@
       <c r="E112" s="12"/>
       <c r="F112"/>
       <c r="G112"/>
-      <c r="H112"/>
-      <c r="I112"/>
       <c r="J112"/>
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.3">
@@ -1812,8 +1583,6 @@
       <c r="E113" s="12"/>
       <c r="F113"/>
       <c r="G113"/>
-      <c r="H113"/>
-      <c r="I113"/>
       <c r="J113"/>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.3">
@@ -1823,8 +1592,6 @@
       <c r="E114" s="12"/>
       <c r="F114"/>
       <c r="G114"/>
-      <c r="H114"/>
-      <c r="I114"/>
       <c r="J114"/>
     </row>
     <row r="115" spans="2:10" x14ac:dyDescent="0.3">
@@ -1834,8 +1601,6 @@
       <c r="E115" s="12"/>
       <c r="F115"/>
       <c r="G115"/>
-      <c r="H115"/>
-      <c r="I115"/>
       <c r="J115"/>
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.3">
@@ -1845,8 +1610,6 @@
       <c r="E116" s="12"/>
       <c r="F116"/>
       <c r="G116"/>
-      <c r="H116"/>
-      <c r="I116"/>
       <c r="J116"/>
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.3">
@@ -1856,8 +1619,6 @@
       <c r="E117" s="12"/>
       <c r="F117"/>
       <c r="G117"/>
-      <c r="H117"/>
-      <c r="I117"/>
       <c r="J117"/>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.3">
@@ -1867,8 +1628,6 @@
       <c r="E118" s="12"/>
       <c r="F118"/>
       <c r="G118"/>
-      <c r="H118"/>
-      <c r="I118"/>
       <c r="J118"/>
     </row>
     <row r="119" spans="2:10" x14ac:dyDescent="0.3">
@@ -1878,8 +1637,6 @@
       <c r="E119" s="12"/>
       <c r="F119"/>
       <c r="G119"/>
-      <c r="H119"/>
-      <c r="I119"/>
       <c r="J119"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.3">
@@ -1889,8 +1646,6 @@
       <c r="E120" s="12"/>
       <c r="F120"/>
       <c r="G120"/>
-      <c r="H120"/>
-      <c r="I120"/>
       <c r="J120"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.3">
@@ -1900,8 +1655,6 @@
       <c r="E121" s="12"/>
       <c r="F121"/>
       <c r="G121"/>
-      <c r="H121"/>
-      <c r="I121"/>
       <c r="J121"/>
     </row>
     <row r="122" spans="2:10" x14ac:dyDescent="0.3">
@@ -1911,8 +1664,6 @@
       <c r="E122" s="12"/>
       <c r="F122"/>
       <c r="G122"/>
-      <c r="H122"/>
-      <c r="I122"/>
       <c r="J122"/>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.3">
@@ -1922,8 +1673,6 @@
       <c r="E123" s="12"/>
       <c r="F123"/>
       <c r="G123"/>
-      <c r="H123"/>
-      <c r="I123"/>
       <c r="J123"/>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.3">
@@ -1933,8 +1682,6 @@
       <c r="E124" s="12"/>
       <c r="F124"/>
       <c r="G124"/>
-      <c r="H124"/>
-      <c r="I124"/>
       <c r="J124"/>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.3">
@@ -1944,8 +1691,6 @@
       <c r="E125" s="12"/>
       <c r="F125"/>
       <c r="G125"/>
-      <c r="H125"/>
-      <c r="I125"/>
       <c r="J125"/>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.3">
@@ -1955,8 +1700,6 @@
       <c r="E126" s="12"/>
       <c r="F126"/>
       <c r="G126"/>
-      <c r="H126"/>
-      <c r="I126"/>
       <c r="J126"/>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.3">
@@ -1966,8 +1709,6 @@
       <c r="E127" s="12"/>
       <c r="F127"/>
       <c r="G127"/>
-      <c r="H127"/>
-      <c r="I127"/>
       <c r="J127"/>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.3">
@@ -1977,8 +1718,6 @@
       <c r="E128" s="12"/>
       <c r="F128"/>
       <c r="G128"/>
-      <c r="H128"/>
-      <c r="I128"/>
       <c r="J128"/>
     </row>
     <row r="129" spans="2:10" x14ac:dyDescent="0.3">
@@ -1988,8 +1727,6 @@
       <c r="E129" s="12"/>
       <c r="F129"/>
       <c r="G129"/>
-      <c r="H129"/>
-      <c r="I129"/>
       <c r="J129"/>
     </row>
     <row r="130" spans="2:10" x14ac:dyDescent="0.3">
@@ -1999,8 +1736,6 @@
       <c r="E130" s="12"/>
       <c r="F130"/>
       <c r="G130"/>
-      <c r="H130"/>
-      <c r="I130"/>
       <c r="J130"/>
     </row>
     <row r="131" spans="2:10" x14ac:dyDescent="0.3">
@@ -2010,8 +1745,6 @@
       <c r="E131" s="12"/>
       <c r="F131"/>
       <c r="G131"/>
-      <c r="H131"/>
-      <c r="I131"/>
       <c r="J131"/>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.3">
@@ -2021,8 +1754,6 @@
       <c r="E132" s="12"/>
       <c r="F132"/>
       <c r="G132"/>
-      <c r="H132"/>
-      <c r="I132"/>
       <c r="J132"/>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.3">
@@ -2032,8 +1763,6 @@
       <c r="E133" s="12"/>
       <c r="F133"/>
       <c r="G133"/>
-      <c r="H133"/>
-      <c r="I133"/>
       <c r="J133"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.3">
@@ -2043,8 +1772,6 @@
       <c r="E134" s="12"/>
       <c r="F134"/>
       <c r="G134"/>
-      <c r="H134"/>
-      <c r="I134"/>
       <c r="J134"/>
     </row>
     <row r="135" spans="2:10" x14ac:dyDescent="0.3">
@@ -2054,8 +1781,6 @@
       <c r="E135" s="12"/>
       <c r="F135"/>
       <c r="G135"/>
-      <c r="H135"/>
-      <c r="I135"/>
       <c r="J135"/>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.3">
@@ -2065,8 +1790,6 @@
       <c r="E136" s="12"/>
       <c r="F136"/>
       <c r="G136"/>
-      <c r="H136"/>
-      <c r="I136"/>
       <c r="J136"/>
     </row>
   </sheetData>
@@ -2074,10 +1797,10 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exchange" prompt="Please select exchange from dropdown list" xr:uid="{FDA4A053-4AB0-48B0-9CA3-6E8174E0D4D6}">
           <x14:formula1>
-            <xm:f>ListOfValues!$A$2:$A$3</xm:f>
+            <xm:f>ListOfValues!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -2104,7 +1827,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2158,7 +1881,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Added testnet feature for ByBit2.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1554B86-3CCA-4DB4-82F5-B6498BFCC552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6828A9-0DC1-400E-8A1C-421B4140C2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1548" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,13 +585,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="12">
-        <v>44440</v>
+        <v>44501</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -603,7 +603,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Set ByBit2 for futures markets.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6828A9-0DC1-400E-8A1C-421B4140C2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFCE228-F961-4205-9708-72944518343B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1548" yWindow="2580" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="2064" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed bug in ScalpingEmaRsiAdx where we were entering trades with signal that occured during precedent trade.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFCE228-F961-4205-9708-72944518343B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6DA502-FBED-44F9-8FFA-22A67022C621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="2064" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -46,15 +46,6 @@
     <t>Test #</t>
   </si>
   <si>
-    <t>Precision Crossing</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>Exchange</t>
   </si>
   <si>
@@ -73,58 +64,64 @@
     <t>Binance</t>
   </si>
   <si>
+    <t>EarlyMACD</t>
+  </si>
+  <si>
+    <t>Pair</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>5m</t>
+  </si>
+  <si>
+    <t>15m</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>1w</t>
+  </si>
+  <si>
+    <t>Initial Capital</t>
+  </si>
+  <si>
+    <t>ScalpingEmaRsiAdx</t>
+  </si>
+  <si>
+    <t>Pairs</t>
+  </si>
+  <si>
     <t>BTCUSDT</t>
   </si>
   <si>
-    <t>EarlyMACD</t>
-  </si>
-  <si>
-    <t>Pair</t>
-  </si>
-  <si>
-    <t>1m</t>
-  </si>
-  <si>
-    <t>3m</t>
-  </si>
-  <si>
-    <t>5m</t>
-  </si>
-  <si>
-    <t>15m</t>
-  </si>
-  <si>
-    <t>30m</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>4h</t>
-  </si>
-  <si>
-    <t>6h</t>
-  </si>
-  <si>
-    <t>12h</t>
-  </si>
-  <si>
-    <t>1d</t>
-  </si>
-  <si>
-    <t>1w</t>
-  </si>
-  <si>
-    <t>Initial Capital</t>
-  </si>
-  <si>
-    <t>ScalpingEmaRsiAdx</t>
-  </si>
-  <si>
-    <t>ByBit2</t>
+    <t>Kraken</t>
+  </si>
+  <si>
+    <t>BTC/USDT</t>
   </si>
 </sst>
 </file>
@@ -524,16 +521,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J136"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" style="1" customWidth="1"/>
     <col min="4" max="5" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
@@ -547,10 +544,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>1</v>
@@ -562,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>3</v>
@@ -571,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -579,31 +576,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D2" s="12">
         <v>44501</v>
       </c>
       <c r="E2" s="12">
-        <v>44561</v>
+        <v>44523</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
       </c>
       <c r="H2" s="8">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="I2" s="8">
-        <v>2.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -619,8 +616,13 @@
       <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="J6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
@@ -1783,24 +1785,15 @@
       <c r="G135"/>
       <c r="J135"/>
     </row>
-    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B136" s="1"/>
-      <c r="C136"/>
-      <c r="D136" s="12"/>
-      <c r="E136" s="12"/>
-      <c r="F136"/>
-      <c r="G136"/>
-      <c r="J136"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exchange" prompt="Please select exchange from dropdown list" xr:uid="{FDA4A053-4AB0-48B0-9CA3-6E8174E0D4D6}">
           <x14:formula1>
-            <xm:f>ListOfValues!$A$2:$A$4</xm:f>
+            <xm:f>ListOfValues!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -1816,6 +1809,12 @@
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Pair" prompt="Please select a pair from the dropdown menu" xr:uid="{75A0F4A4-B460-4AB8-ABE3-AF589BA63307}">
+          <x14:formula1>
+            <xm:f>ListOfValues!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1827,7 +1826,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1840,110 +1839,110 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Enter/Exit statuses on the same line.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC219F14-1585-4A00-B8B6-A9F48D536DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8818F81F-DD2B-4C10-A5DD-B0843725C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="528" yWindow="2412" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,13 +580,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="12">
-        <v>44378</v>
+        <v>44501</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -598,7 +598,7 @@
         <v>10000</v>
       </c>
       <c r="H2" s="8">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="8">
         <v>1</v>
@@ -618,7 +618,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="12">
-        <v>44378</v>
+        <v>44501</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
@@ -630,78 +630,22 @@
         <v>10000</v>
       </c>
       <c r="H3" s="8">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="8">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="12">
-        <v>44378</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="12">
-        <v>44378</v>
-      </c>
-      <c r="E5" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>

</xml_diff>

<commit_message>
Added support for saving/reading historical data in PostgreSQL local database.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8818F81F-DD2B-4C10-A5DD-B0843725C1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0954AE-55C3-4C3C-A427-1ECDDE7D20AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="876" yWindow="2760" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Exchanges</t>
   </si>
   <si>
-    <t>ByBit</t>
-  </si>
-  <si>
     <t>Strategy</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>ScalpEmaRsiAdx</t>
+  </si>
+  <si>
+    <t>Bybit</t>
   </si>
 </sst>
 </file>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J133"/>
+  <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>1</v>
@@ -563,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>3</v>
@@ -572,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -580,19 +580,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44501</v>
+        <v>44197</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -604,27 +604,27 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="12">
-        <v>44501</v>
+        <v>44197</v>
       </c>
       <c r="E3" s="12">
         <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -644,8 +644,13 @@
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
@@ -1789,15 +1794,6 @@
       <c r="F132"/>
       <c r="G132"/>
       <c r="J132"/>
-    </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B133" s="1"/>
-      <c r="C133"/>
-      <c r="D133" s="12"/>
-      <c r="E133" s="12"/>
-      <c r="F133"/>
-      <c r="G133"/>
-      <c r="J133"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1834,7 +1830,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1850,107 +1846,107 @@
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a few details regrading database import process.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0954AE-55C3-4C3C-A427-1ECDDE7D20AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0095C6-96EE-4D7C-A3AE-1EC823C3D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="876" yWindow="2760" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
@@ -608,36 +608,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="12">
-        <v>44197</v>
-      </c>
-      <c r="E3" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" s="12"/>

</xml_diff>

<commit_message>
Added Details column in the statistics.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0095C6-96EE-4D7C-A3AE-1EC823C3D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE357B-9E5C-4C5A-BE91-BEBA95BF4A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="876" yWindow="2760" windowWidth="20460" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J132"/>
+  <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +586,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44197</v>
+        <v>44531</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
@@ -598,10 +598,10 @@
         <v>10000</v>
       </c>
       <c r="H2" s="8">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="I2" s="8">
-        <v>1</v>
+        <v>0.83</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>29</v>
@@ -612,8 +612,13 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1757,15 +1762,6 @@
       <c r="F131"/>
       <c r="G131"/>
       <c r="J131"/>
-    </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B132" s="1"/>
-      <c r="C132"/>
-      <c r="D132" s="12"/>
-      <c r="E132" s="12"/>
-      <c r="F132"/>
-      <c r="G132"/>
-      <c r="J132"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
In database mode statistics results are also stored in the db.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DE357B-9E5C-4C5A-BE91-BEBA95BF4A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5861020D-4780-490A-A561-544F81B00603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,13 +586,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44531</v>
+        <v>44501</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -608,17 +608,68 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="12">
+        <v>44501</v>
+      </c>
+      <c r="E3" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="J4"/>
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="12">
+        <v>44501</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
Added tweaker to reduce execution speed for _X strategies.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5861020D-4780-490A-A561-544F81B00603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35747CC5-7143-4A7A-AEC3-4F4750ADF865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1224" windowWidth="15432" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J131"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,13 +586,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44501</v>
+        <v>44197</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -608,68 +608,22 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="12">
-        <v>44501</v>
-      </c>
-      <c r="E3" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="12">
-        <v>44501</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1795,24 +1749,6 @@
       <c r="F129"/>
       <c r="G129"/>
       <c r="J129"/>
-    </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B130" s="1"/>
-      <c r="C130"/>
-      <c r="D130" s="12"/>
-      <c r="E130" s="12"/>
-      <c r="F130"/>
-      <c r="G130"/>
-      <c r="J130"/>
-    </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B131" s="1"/>
-      <c r="C131"/>
-      <c r="D131" s="12"/>
-      <c r="E131" s="12"/>
-      <c r="F131"/>
-      <c r="G131"/>
-      <c r="J131"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Disabled tweak that is not working in _X strategies.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35747CC5-7143-4A7A-AEC3-4F4750ADF865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F329318C-D437-4D16-BD7A-4FBDEF939D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1224" windowWidth="15432" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1632" yWindow="2208" windowWidth="19356" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,7 +586,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44197</v>
+        <v>44470</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>

</xml_diff>

<commit_message>
Removed tweak for -X strategies that pass smaller dataframes to in-minute method.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F329318C-D437-4D16-BD7A-4FBDEF939D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900A5D90-7A02-495D-A377-93754DD9860F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1632" yWindow="2208" windowWidth="19356" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,13 +586,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="E2" s="12">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -604,17 +604,40 @@
         <v>0.83</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="12">
+        <v>44531</v>
+      </c>
+      <c r="E3" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>

</xml_diff>

<commit_message>
Fixed details column output in statistics.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900A5D90-7A02-495D-A377-93754DD9860F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46159252-E2FD-4A22-A464-A6BE2FE6CEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1632" yWindow="2208" windowWidth="19356" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J129"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,13 +586,13 @@
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44531</v>
+        <v>43831</v>
       </c>
       <c r="E2" s="12">
-        <v>44561</v>
+        <v>44196</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="8">
         <v>10000</v>
@@ -604,7 +604,7 @@
         <v>0.83</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -615,16 +615,16 @@
         <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="12">
-        <v>44531</v>
+        <v>43831</v>
       </c>
       <c r="E3" s="12">
-        <v>44561</v>
+        <v>44196</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="8">
         <v>10000</v>
@@ -640,22 +640,68 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="J4"/>
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="12">
+        <v>44197</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="J5"/>
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="12">
+        <v>44197</v>
+      </c>
+      <c r="E5" s="12">
+        <v>44561</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
@@ -1763,15 +1809,6 @@
       <c r="F128"/>
       <c r="G128"/>
       <c r="J128"/>
-    </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B129" s="1"/>
-      <c r="C129"/>
-      <c r="D129" s="12"/>
-      <c r="E129" s="12"/>
-      <c r="F129"/>
-      <c r="G129"/>
-      <c r="J129"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1808,7 +1845,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1837,9 +1874,7 @@
       <c r="A2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2" s="15"/>
       <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1852,7 +1887,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>13</v>
@@ -1864,7 +1899,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>14</v>
@@ -1873,14 +1908,16 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
+      <c r="B6" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Fixed bug with fees when entering trades as taker.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46159252-E2FD-4A22-A464-A6BE2FE6CEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEDF9A4-1682-4D2A-AB5C-12840D1BE234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1632" yWindow="2208" windowWidth="19356" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,16 +580,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>43831</v>
+        <v>44501</v>
       </c>
       <c r="E2" s="12">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -615,13 +615,13 @@
         <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="12">
-        <v>43831</v>
+        <v>44501</v>
       </c>
       <c r="E3" s="12">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
@@ -640,68 +640,22 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="12">
-        <v>44197</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="8">
-        <v>0.83</v>
-      </c>
-      <c r="I4" s="8">
-        <v>0.83</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="J4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="12">
-        <v>44197</v>
-      </c>
-      <c r="E5" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0.83</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.83</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
@@ -1782,33 +1736,6 @@
       <c r="F125"/>
       <c r="G125"/>
       <c r="J125"/>
-    </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B126" s="1"/>
-      <c r="C126"/>
-      <c r="D126" s="12"/>
-      <c r="E126" s="12"/>
-      <c r="F126"/>
-      <c r="G126"/>
-      <c r="J126"/>
-    </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B127" s="1"/>
-      <c r="C127"/>
-      <c r="D127" s="12"/>
-      <c r="E127" s="12"/>
-      <c r="F127"/>
-      <c r="G127"/>
-      <c r="J127"/>
-    </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B128" s="1"/>
-      <c r="C128"/>
-      <c r="D128" s="12"/>
-      <c r="E128" s="12"/>
-      <c r="F128"/>
-      <c r="G128"/>
-      <c r="J128"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added strategy details in console output.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEDF9A4-1682-4D2A-AB5C-12840D1BE234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28D5566-B75A-42A5-9784-E955DA7C9292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1632" yWindow="2208" windowWidth="19356" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +604,7 @@
         <v>0.83</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -636,7 +636,7 @@
         <v>0.83</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added EMA_TOLERANCE changes to the ScalpEmaRsiAdx_X strategy.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749620DF-2AB1-4C7D-9373-3E15BE18BFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB09AE8-8C1E-425A-B15A-A721EE66FCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5310" yWindow="2160" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="1770" windowWidth="19260" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,40 +604,17 @@
         <v>0.23</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="12">
-        <v>44501</v>
-      </c>
-      <c r="E3" s="12">
-        <v>44561</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="J3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -1718,15 +1695,6 @@
       <c r="F123"/>
       <c r="G123"/>
       <c r="J123"/>
-    </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B124" s="1"/>
-      <c r="C124"/>
-      <c r="D124" s="12"/>
-      <c r="E124" s="12"/>
-      <c r="F124"/>
-      <c r="G124"/>
-      <c r="J124"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed ESI bug in _X strategies.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB09AE8-8C1E-425A-B15A-A721EE66FCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E52F0-48CD-408F-B362-A5DEB72DC36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="1770" windowWidth="19260" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="3465" windowWidth="27390" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,16 +580,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="12">
-        <v>44501</v>
+        <v>44579</v>
       </c>
       <c r="E2" s="12">
-        <v>44561</v>
+        <v>44586</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -601,7 +601,7 @@
         <v>0.3</v>
       </c>
       <c r="I2" s="8">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Changeconfiguration to use config.json.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E52F0-48CD-408F-B362-A5DEB72DC36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBB8973-0A8D-48E1-8DEE-984CC7E25E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="3465" windowWidth="27390" windowHeight="9150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18405" yWindow="1095" windowWidth="18720" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Interval</t>
   </si>
@@ -527,7 +527,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,35 +604,104 @@
         <v>0.2</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="12">
+        <v>44579</v>
+      </c>
+      <c r="E3" s="12">
+        <v>44586</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="12">
+        <v>44579</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44586</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="12">
+        <v>44579</v>
+      </c>
+      <c r="E5" s="12">
+        <v>44586</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="8">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="J5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>

</xml_diff>

<commit_message>
Fixed bug missing tp/sl trade exits.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD520096-C3F2-419C-B268-0594C2742F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDAD27A-009B-4C5A-93E2-D2AC66431AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="2790" windowWidth="25695" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="19290" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Interval</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>MACD_BB_Freeman</t>
+  </si>
+  <si>
+    <t>Exit Strategy</t>
+  </si>
+  <si>
+    <t>ExitOnNextEntry</t>
+  </si>
+  <si>
+    <t>FixedPCT</t>
+  </si>
+  <si>
+    <t>Exit_Strategy</t>
   </si>
 </sst>
 </file>
@@ -202,15 +214,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -228,22 +234,25 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,33 +535,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.85546875" style="8" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="12" t="s">
@@ -561,221 +572,131 @@
       <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="K1" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="14">
-        <v>44197</v>
-      </c>
-      <c r="E2" s="14">
-        <v>44594</v>
+      <c r="D2" s="10">
+        <v>44459</v>
+      </c>
+      <c r="E2" s="10">
+        <v>44593</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="6">
         <v>10000</v>
       </c>
-      <c r="H2" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I2" s="8">
-        <v>1.1000000000000001</v>
+      <c r="H2" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.8</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="14">
-        <v>44197</v>
-      </c>
-      <c r="E3" s="14">
-        <v>44594</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="14">
-        <v>44197</v>
-      </c>
-      <c r="E4" s="14">
-        <v>44594</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I4" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="14">
-        <v>44197</v>
-      </c>
-      <c r="E5" s="14">
-        <v>44594</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="8">
-        <v>10000</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="J7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8"/>
       <c r="F8"/>
       <c r="G8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9"/>
       <c r="F9"/>
       <c r="G9"/>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10"/>
       <c r="F10"/>
       <c r="G10"/>
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11"/>
       <c r="F11"/>
       <c r="G11"/>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13"/>
       <c r="F13"/>
       <c r="G13"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15"/>
       <c r="F15"/>
       <c r="G15"/>
       <c r="J15"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16"/>
       <c r="F16"/>
@@ -1515,7 +1436,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exchange" prompt="Please select exchange from dropdown list" xr:uid="{FDA4A053-4AB0-48B0-9CA3-6E8174E0D4D6}">
           <x14:formula1>
             <xm:f>ListOfValues!$A$2:$A$5</xm:f>
@@ -1530,7 +1451,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Interval" prompt="Please select interval from dropdown list" xr:uid="{B01186AF-2E82-4CE1-BAFD-D7EED7D3D148}">
           <x14:formula1>
-            <xm:f>ListOfValues!$C$2:$C$13</xm:f>
+            <xm:f>ListOfValues!$D$2:$D$13</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
@@ -1539,6 +1460,12 @@
             <xm:f>ListOfValues!$E$2:$E$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exit Strategy" prompt="Please select the way trades exit from the dropdown list" xr:uid="{3B7B2715-8F43-4FA9-A6F2-16C54D666CE1}">
+          <x14:formula1>
+            <xm:f>ListOfValues!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1551,126 +1478,146 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1"/>
     <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ExitOnNextEntry mode and fixed bugs on trade entries for ScalpEmaRsiAdx.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDAD27A-009B-4C5A-93E2-D2AC66431AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED858591-5E24-47EB-A6E5-7196EA03F607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19290" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28950" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Interval</t>
   </si>
@@ -538,7 +538,7 @@
   <dimension ref="A1:K120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="10">
-        <v>44459</v>
+        <v>44550</v>
       </c>
       <c r="E2" s="10">
         <v>44593</v>
@@ -614,24 +614,157 @@
         <v>10000</v>
       </c>
       <c r="H2" s="6">
-        <v>0.8</v>
+        <v>4</v>
       </c>
       <c r="I2" s="6">
-        <v>0.8</v>
+        <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="10">
+        <v>44550</v>
+      </c>
+      <c r="E3" s="10">
+        <v>44593</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="10">
+        <v>44550</v>
+      </c>
+      <c r="E4" s="10">
+        <v>44593</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="10">
+        <v>44550</v>
+      </c>
+      <c r="E5" s="10">
+        <v>44593</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="10">
+        <v>44550</v>
+      </c>
+      <c r="E6" s="10">
+        <v>44593</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="J6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -1478,7 +1611,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added order by clause when pulling candle data from db.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E7DB2D-9DB5-4D8D-883D-DDEB9498884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3874C2F-8F48-46B5-BE9B-DE256C959F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20955" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9345" yWindow="5445" windowWidth="20955" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +599,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="10">
-        <v>44531</v>
+        <v>44470</v>
       </c>
       <c r="E2" s="10">
-        <v>44593</v>
+        <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -614,10 +614,10 @@
         <v>10000</v>
       </c>
       <c r="H2" s="6">
-        <v>1.5</v>
+        <v>19</v>
       </c>
       <c r="I2" s="6">
-        <v>1.5</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Added option1 and option2 in TestCases.xlsx.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3874C2F-8F48-46B5-BE9B-DE256C959F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D23A7D-DCEB-4C75-9F7B-02B69E2153E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9345" yWindow="5445" windowWidth="20955" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11640" yWindow="2850" windowWidth="20880" windowHeight="12915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Interval</t>
   </si>
@@ -100,9 +100,6 @@
     <t>1w</t>
   </si>
   <si>
-    <t>Initial Capital</t>
-  </si>
-  <si>
     <t>Pairs</t>
   </si>
   <si>
@@ -137,6 +134,24 @@
   </si>
   <si>
     <t>Exit_Strategy</t>
+  </si>
+  <si>
+    <t>Option1</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>EMA</t>
+  </si>
+  <si>
+    <t>WMA</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Option2</t>
   </si>
 </sst>
 </file>
@@ -174,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -210,11 +225,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,9 +263,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -253,6 +276,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -535,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,876 +575,802 @@
     <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
+    <col min="11" max="12" width="12.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="J1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="10">
-        <v>44470</v>
-      </c>
-      <c r="E2" s="10">
+        <v>26</v>
+      </c>
+      <c r="D2" s="9">
+        <v>44531</v>
+      </c>
+      <c r="E2" s="9">
         <v>44561</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>10000</v>
+        <v>1.2</v>
       </c>
       <c r="H2" s="6">
-        <v>19</v>
-      </c>
-      <c r="I2" s="6">
-        <v>19</v>
+        <v>1.2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="9">
+        <v>44531</v>
+      </c>
+      <c r="E3" s="9">
+        <v>44561</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6"/>
       <c r="F6"/>
-      <c r="G6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7"/>
       <c r="F7"/>
-      <c r="G7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8"/>
       <c r="F8"/>
-      <c r="G8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9"/>
       <c r="F9"/>
-      <c r="G9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10"/>
       <c r="F10"/>
-      <c r="G10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11"/>
       <c r="F11"/>
-      <c r="G11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12"/>
       <c r="F12"/>
-      <c r="G12"/>
-      <c r="J12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13"/>
       <c r="F13"/>
-      <c r="G13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14"/>
       <c r="F14"/>
-      <c r="G14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15"/>
       <c r="F15"/>
-      <c r="G15"/>
-      <c r="J15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16"/>
       <c r="F16"/>
-      <c r="G16"/>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17"/>
       <c r="F17"/>
-      <c r="G17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18"/>
       <c r="F18"/>
-      <c r="G18"/>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19"/>
       <c r="F19"/>
-      <c r="G19"/>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I19"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20"/>
       <c r="F20"/>
-      <c r="G20"/>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21"/>
       <c r="F21"/>
-      <c r="G21"/>
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22"/>
       <c r="F22"/>
-      <c r="G22"/>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23"/>
       <c r="F23"/>
-      <c r="G23"/>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I23"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24"/>
       <c r="F24"/>
-      <c r="G24"/>
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I24"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25"/>
       <c r="F25"/>
-      <c r="G25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I25"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26"/>
       <c r="F26"/>
-      <c r="G26"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I26"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27"/>
       <c r="F27"/>
-      <c r="G27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28"/>
       <c r="F28"/>
-      <c r="G28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I28"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29"/>
       <c r="F29"/>
-      <c r="G29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I29"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30"/>
       <c r="F30"/>
-      <c r="G30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31"/>
       <c r="F31"/>
-      <c r="G31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32"/>
       <c r="F32"/>
-      <c r="G32"/>
-      <c r="J32"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33"/>
       <c r="F33"/>
-      <c r="G33"/>
-      <c r="J33"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34"/>
       <c r="F34"/>
-      <c r="G34"/>
-      <c r="J34"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35"/>
       <c r="F35"/>
-      <c r="G35"/>
-      <c r="J35"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36"/>
       <c r="F36"/>
-      <c r="G36"/>
-      <c r="J36"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I36"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37"/>
       <c r="F37"/>
-      <c r="G37"/>
-      <c r="J37"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I37"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38"/>
       <c r="F38"/>
-      <c r="G38"/>
-      <c r="J38"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I38"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39"/>
       <c r="F39"/>
-      <c r="G39"/>
-      <c r="J39"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40"/>
       <c r="F40"/>
-      <c r="G40"/>
-      <c r="J40"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41"/>
       <c r="F41"/>
-      <c r="G41"/>
-      <c r="J41"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42"/>
       <c r="F42"/>
-      <c r="G42"/>
-      <c r="J42"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43"/>
       <c r="F43"/>
-      <c r="G43"/>
-      <c r="J43"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44"/>
       <c r="F44"/>
-      <c r="G44"/>
-      <c r="J44"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45"/>
       <c r="F45"/>
-      <c r="G45"/>
-      <c r="J45"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46"/>
       <c r="F46"/>
-      <c r="G46"/>
-      <c r="J46"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47"/>
       <c r="F47"/>
-      <c r="G47"/>
-      <c r="J47"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48"/>
       <c r="F48"/>
-      <c r="G48"/>
-      <c r="J48"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49"/>
       <c r="F49"/>
-      <c r="G49"/>
-      <c r="J49"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50"/>
       <c r="F50"/>
-      <c r="G50"/>
-      <c r="J50"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51"/>
       <c r="F51"/>
-      <c r="G51"/>
-      <c r="J51"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52"/>
       <c r="F52"/>
-      <c r="G52"/>
-      <c r="J52"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53"/>
       <c r="F53"/>
-      <c r="G53"/>
-      <c r="J53"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54"/>
       <c r="F54"/>
-      <c r="G54"/>
-      <c r="J54"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55"/>
       <c r="F55"/>
-      <c r="G55"/>
-      <c r="J55"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I55"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56"/>
       <c r="F56"/>
-      <c r="G56"/>
-      <c r="J56"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57"/>
       <c r="F57"/>
-      <c r="G57"/>
-      <c r="J57"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58"/>
       <c r="F58"/>
-      <c r="G58"/>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59"/>
       <c r="F59"/>
-      <c r="G59"/>
-      <c r="J59"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60"/>
       <c r="F60"/>
-      <c r="G60"/>
-      <c r="J60"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61"/>
       <c r="F61"/>
-      <c r="G61"/>
-      <c r="J61"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I61"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62"/>
       <c r="F62"/>
-      <c r="G62"/>
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63"/>
       <c r="F63"/>
-      <c r="G63"/>
-      <c r="J63"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64"/>
       <c r="F64"/>
-      <c r="G64"/>
-      <c r="J64"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65"/>
       <c r="F65"/>
-      <c r="G65"/>
-      <c r="J65"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I65"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66"/>
       <c r="F66"/>
-      <c r="G66"/>
-      <c r="J66"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I66"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67"/>
       <c r="F67"/>
-      <c r="G67"/>
-      <c r="J67"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I67"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68"/>
       <c r="F68"/>
-      <c r="G68"/>
-      <c r="J68"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I68"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69"/>
       <c r="F69"/>
-      <c r="G69"/>
-      <c r="J69"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I69"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70"/>
       <c r="F70"/>
-      <c r="G70"/>
-      <c r="J70"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I70"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71"/>
       <c r="F71"/>
-      <c r="G71"/>
-      <c r="J71"/>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I71"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72"/>
       <c r="F72"/>
-      <c r="G72"/>
-      <c r="J72"/>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I72"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73"/>
       <c r="F73"/>
-      <c r="G73"/>
-      <c r="J73"/>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I73"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74"/>
       <c r="F74"/>
-      <c r="G74"/>
-      <c r="J74"/>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I74"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75"/>
       <c r="F75"/>
-      <c r="G75"/>
-      <c r="J75"/>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I75"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76"/>
       <c r="F76"/>
-      <c r="G76"/>
-      <c r="J76"/>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I76"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77"/>
       <c r="F77"/>
-      <c r="G77"/>
-      <c r="J77"/>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78"/>
       <c r="F78"/>
-      <c r="G78"/>
-      <c r="J78"/>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79"/>
       <c r="F79"/>
-      <c r="G79"/>
-      <c r="J79"/>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I79"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80"/>
       <c r="F80"/>
-      <c r="G80"/>
-      <c r="J80"/>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I80"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81"/>
       <c r="F81"/>
-      <c r="G81"/>
-      <c r="J81"/>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I81"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82"/>
       <c r="F82"/>
-      <c r="G82"/>
-      <c r="J82"/>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83"/>
       <c r="F83"/>
-      <c r="G83"/>
-      <c r="J83"/>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84"/>
       <c r="F84"/>
-      <c r="G84"/>
-      <c r="J84"/>
-    </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85"/>
       <c r="F85"/>
-      <c r="G85"/>
-      <c r="J85"/>
-    </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I85"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86"/>
       <c r="F86"/>
-      <c r="G86"/>
-      <c r="J86"/>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I86"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87"/>
       <c r="F87"/>
-      <c r="G87"/>
-      <c r="J87"/>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I87"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88"/>
       <c r="F88"/>
-      <c r="G88"/>
-      <c r="J88"/>
-    </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I88"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89"/>
       <c r="F89"/>
-      <c r="G89"/>
-      <c r="J89"/>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I89"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90"/>
       <c r="F90"/>
-      <c r="G90"/>
-      <c r="J90"/>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I90"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91"/>
       <c r="F91"/>
-      <c r="G91"/>
-      <c r="J91"/>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I91"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92"/>
       <c r="F92"/>
-      <c r="G92"/>
-      <c r="J92"/>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I92"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93"/>
       <c r="F93"/>
-      <c r="G93"/>
-      <c r="J93"/>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I93"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94"/>
       <c r="F94"/>
-      <c r="G94"/>
-      <c r="J94"/>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I94"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95"/>
       <c r="F95"/>
-      <c r="G95"/>
-      <c r="J95"/>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I95"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96"/>
       <c r="F96"/>
-      <c r="G96"/>
-      <c r="J96"/>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I96"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97"/>
       <c r="F97"/>
-      <c r="G97"/>
-      <c r="J97"/>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I97"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98"/>
       <c r="F98"/>
-      <c r="G98"/>
-      <c r="J98"/>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I98"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99"/>
       <c r="F99"/>
-      <c r="G99"/>
-      <c r="J99"/>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I99"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100"/>
       <c r="F100"/>
-      <c r="G100"/>
-      <c r="J100"/>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I100"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101"/>
       <c r="F101"/>
-      <c r="G101"/>
-      <c r="J101"/>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I101"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102"/>
       <c r="F102"/>
-      <c r="G102"/>
-      <c r="J102"/>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I102"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103"/>
       <c r="F103"/>
-      <c r="G103"/>
-      <c r="J103"/>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I103"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104"/>
       <c r="F104"/>
-      <c r="G104"/>
-      <c r="J104"/>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I104"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105"/>
       <c r="F105"/>
-      <c r="G105"/>
-      <c r="J105"/>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I105"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106"/>
       <c r="F106"/>
-      <c r="G106"/>
-      <c r="J106"/>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I106"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107"/>
       <c r="F107"/>
-      <c r="G107"/>
-      <c r="J107"/>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I107"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108"/>
       <c r="F108"/>
-      <c r="G108"/>
-      <c r="J108"/>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I108"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109"/>
       <c r="F109"/>
-      <c r="G109"/>
-      <c r="J109"/>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I109"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110"/>
       <c r="F110"/>
-      <c r="G110"/>
-      <c r="J110"/>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I110"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111"/>
       <c r="F111"/>
-      <c r="G111"/>
-      <c r="J111"/>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I111"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112"/>
       <c r="F112"/>
-      <c r="G112"/>
-      <c r="J112"/>
-    </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I112"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="C113"/>
       <c r="F113"/>
-      <c r="G113"/>
-      <c r="J113"/>
-    </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I113"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114"/>
       <c r="F114"/>
-      <c r="G114"/>
-      <c r="J114"/>
-    </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I114"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115"/>
       <c r="F115"/>
-      <c r="G115"/>
-      <c r="J115"/>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I115"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116"/>
       <c r="F116"/>
-      <c r="G116"/>
-      <c r="J116"/>
-    </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I116"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117"/>
       <c r="F117"/>
-      <c r="G117"/>
-      <c r="J117"/>
+      <c r="I117"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exchange" prompt="Please select exchange from dropdown list" xr:uid="{FDA4A053-4AB0-48B0-9CA3-6E8174E0D4D6}">
           <x14:formula1>
             <xm:f>ListOfValues!$A$2:$A$5</xm:f>
@@ -1426,7 +1381,7 @@
           <x14:formula1>
             <xm:f>ListOfValues!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Interval" prompt="Please select interval from dropdown list" xr:uid="{B01186AF-2E82-4CE1-BAFD-D7EED7D3D148}">
           <x14:formula1>
@@ -1444,6 +1399,12 @@
           <x14:formula1>
             <xm:f>ListOfValues!$C$2:$C$3</xm:f>
           </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman you can pick the moving average type in the drop down menu" xr:uid="{96A1433D-0EEB-474D-93F6-A823D5795C69}">
+          <x14:formula1>
+            <xm:f>ListOfValues!$F$2:$F$6</xm:f>
+          </x14:formula1>
           <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
@@ -1454,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{183ECDD1-3B17-49FC-A8D8-202F644155E1}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,9 +1428,10 @@
     <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1"/>
     <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1477,128 +1439,167 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>32</v>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
-        <v>30</v>
+      <c r="F4" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>29</v>
+      <c r="F5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Made Option2 link to ADX for the MACD_BB_FReeman strategy.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D23A7D-DCEB-4C75-9F7B-02B69E2153E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC8531D-AF18-44A0-97B5-62CB905615AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="2850" windowWidth="20880" windowHeight="12915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11400" yWindow="1365" windowWidth="18315" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Interval</t>
   </si>
@@ -240,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,6 +283,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +585,8 @@
     <col min="8" max="8" width="8.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="12.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -619,7 +623,7 @@
       <c r="K1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>41</v>
       </c>
     </row>
@@ -634,19 +638,19 @@
         <v>26</v>
       </c>
       <c r="D2" s="9">
-        <v>44531</v>
+        <v>44228</v>
       </c>
       <c r="E2" s="9">
-        <v>44561</v>
+        <v>44620</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="H2" s="6">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>31</v>
@@ -659,39 +663,22 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="9">
-        <v>44531</v>
-      </c>
-      <c r="E3" s="9">
-        <v>44561</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3"/>
+      <c r="F3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4"/>
+      <c r="F4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5"/>
+      <c r="F5"/>
+      <c r="I5"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -969,408 +956,26 @@
       <c r="F51"/>
       <c r="I51"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52"/>
-      <c r="F52"/>
-      <c r="I52"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53"/>
-      <c r="F53"/>
-      <c r="I53"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54"/>
-      <c r="F54"/>
-      <c r="I54"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55"/>
-      <c r="F55"/>
-      <c r="I55"/>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56"/>
-      <c r="F56"/>
-      <c r="I56"/>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57"/>
-      <c r="F57"/>
-      <c r="I57"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58"/>
-      <c r="F58"/>
-      <c r="I58"/>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59"/>
-      <c r="F59"/>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60"/>
-      <c r="F60"/>
-      <c r="I60"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="C61"/>
-      <c r="F61"/>
-      <c r="I61"/>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-      <c r="C62"/>
-      <c r="F62"/>
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63"/>
-      <c r="F63"/>
-      <c r="I63"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="C64"/>
-      <c r="F64"/>
-      <c r="I64"/>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="C65"/>
-      <c r="F65"/>
-      <c r="I65"/>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="C66"/>
-      <c r="F66"/>
-      <c r="I66"/>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67"/>
-      <c r="F67"/>
-      <c r="I67"/>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-      <c r="C68"/>
-      <c r="F68"/>
-      <c r="I68"/>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="C69"/>
-      <c r="F69"/>
-      <c r="I69"/>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-      <c r="C70"/>
-      <c r="F70"/>
-      <c r="I70"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-      <c r="C71"/>
-      <c r="F71"/>
-      <c r="I71"/>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-      <c r="C72"/>
-      <c r="F72"/>
-      <c r="I72"/>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-      <c r="C73"/>
-      <c r="F73"/>
-      <c r="I73"/>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-      <c r="C74"/>
-      <c r="F74"/>
-      <c r="I74"/>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-      <c r="C75"/>
-      <c r="F75"/>
-      <c r="I75"/>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
-      <c r="C76"/>
-      <c r="F76"/>
-      <c r="I76"/>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-      <c r="C77"/>
-      <c r="F77"/>
-      <c r="I77"/>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
-      <c r="C78"/>
-      <c r="F78"/>
-      <c r="I78"/>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-      <c r="C79"/>
-      <c r="F79"/>
-      <c r="I79"/>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-      <c r="C80"/>
-      <c r="F80"/>
-      <c r="I80"/>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
-      <c r="C81"/>
-      <c r="F81"/>
-      <c r="I81"/>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
-      <c r="C82"/>
-      <c r="F82"/>
-      <c r="I82"/>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
-      <c r="C83"/>
-      <c r="F83"/>
-      <c r="I83"/>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="1"/>
-      <c r="C84"/>
-      <c r="F84"/>
-      <c r="I84"/>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
-      <c r="C85"/>
-      <c r="F85"/>
-      <c r="I85"/>
-    </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
-      <c r="C86"/>
-      <c r="F86"/>
-      <c r="I86"/>
-    </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
-      <c r="C87"/>
-      <c r="F87"/>
-      <c r="I87"/>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="1"/>
-      <c r="C88"/>
-      <c r="F88"/>
-      <c r="I88"/>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
-      <c r="C89"/>
-      <c r="F89"/>
-      <c r="I89"/>
-    </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B90" s="1"/>
-      <c r="C90"/>
-      <c r="F90"/>
-      <c r="I90"/>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="1"/>
-      <c r="C91"/>
-      <c r="F91"/>
-      <c r="I91"/>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B92" s="1"/>
-      <c r="C92"/>
-      <c r="F92"/>
-      <c r="I92"/>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B93" s="1"/>
-      <c r="C93"/>
-      <c r="F93"/>
-      <c r="I93"/>
-    </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="1"/>
-      <c r="C94"/>
-      <c r="F94"/>
-      <c r="I94"/>
-    </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="1"/>
-      <c r="C95"/>
-      <c r="F95"/>
-      <c r="I95"/>
-    </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="1"/>
-      <c r="C96"/>
-      <c r="F96"/>
-      <c r="I96"/>
-    </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B97" s="1"/>
-      <c r="C97"/>
-      <c r="F97"/>
-      <c r="I97"/>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B98" s="1"/>
-      <c r="C98"/>
-      <c r="F98"/>
-      <c r="I98"/>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="1"/>
-      <c r="C99"/>
-      <c r="F99"/>
-      <c r="I99"/>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B100" s="1"/>
-      <c r="C100"/>
-      <c r="F100"/>
-      <c r="I100"/>
-    </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B101" s="1"/>
-      <c r="C101"/>
-      <c r="F101"/>
-      <c r="I101"/>
-    </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="1"/>
-      <c r="C102"/>
-      <c r="F102"/>
-      <c r="I102"/>
-    </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="1"/>
-      <c r="C103"/>
-      <c r="F103"/>
-      <c r="I103"/>
-    </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B104" s="1"/>
-      <c r="C104"/>
-      <c r="F104"/>
-      <c r="I104"/>
-    </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B105" s="1"/>
-      <c r="C105"/>
-      <c r="F105"/>
-      <c r="I105"/>
-    </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B106" s="1"/>
-      <c r="C106"/>
-      <c r="F106"/>
-      <c r="I106"/>
-    </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B107" s="1"/>
-      <c r="C107"/>
-      <c r="F107"/>
-      <c r="I107"/>
-    </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="1"/>
-      <c r="C108"/>
-      <c r="F108"/>
-      <c r="I108"/>
-    </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B109" s="1"/>
-      <c r="C109"/>
-      <c r="F109"/>
-      <c r="I109"/>
-    </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B110" s="1"/>
-      <c r="C110"/>
-      <c r="F110"/>
-      <c r="I110"/>
-    </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B111" s="1"/>
-      <c r="C111"/>
-      <c r="F111"/>
-      <c r="I111"/>
-    </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B112" s="1"/>
-      <c r="C112"/>
-      <c r="F112"/>
-      <c r="I112"/>
-    </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B113" s="1"/>
-      <c r="C113"/>
-      <c r="F113"/>
-      <c r="I113"/>
-    </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B114" s="1"/>
-      <c r="C114"/>
-      <c r="F114"/>
-      <c r="I114"/>
-    </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B115" s="1"/>
-      <c r="C115"/>
-      <c r="F115"/>
-      <c r="I115"/>
-    </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="1"/>
-      <c r="C116"/>
-      <c r="F116"/>
-      <c r="I116"/>
-    </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B117" s="1"/>
-      <c r="C117"/>
-      <c r="F117"/>
-      <c r="I117"/>
-    </row>
   </sheetData>
+  <dataValidations xWindow="923" yWindow="287" count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman this option will override ADX_THRESHOLD field found in the class" sqref="L2:L1048576" xr:uid="{7257D8D3-A242-49AD-A664-6AC115EC7B9B}">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{D812B71D-FF2F-483A-9C34-CCCA6DC36707}">
+      <formula1>1</formula1>
+      <formula2>99999</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 H2:H1048576" xr:uid="{FC39107B-6731-40C3-900C-0A06F0710416}">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="154" yWindow="334" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="923" yWindow="287" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exchange" prompt="Please select exchange from dropdown list" xr:uid="{FDA4A053-4AB0-48B0-9CA3-6E8174E0D4D6}">
           <x14:formula1>
             <xm:f>ListOfValues!$A$2:$A$5</xm:f>
@@ -1401,7 +1006,7 @@
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman you can pick the moving average type in the drop down menu" xr:uid="{96A1433D-0EEB-474D-93F6-A823D5795C69}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman this value will override the MA_CALCULATION_TYPE field in the class" xr:uid="{96A1433D-0EEB-474D-93F6-A823D5795C69}">
           <x14:formula1>
             <xm:f>ListOfValues!$F$2:$F$6</xm:f>
           </x14:formula1>
@@ -1418,14 +1023,14 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1"/>
     <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
@@ -1452,13 +1057,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1472,13 +1077,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -1492,11 +1097,11 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1506,11 +1111,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="8"/>
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
@@ -1520,11 +1125,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1532,9 +1137,9 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1542,9 +1147,9 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1552,9 +1157,9 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1562,9 +1167,9 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1572,9 +1177,9 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1582,9 +1187,9 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
@@ -1592,9 +1197,9 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Fixed fees calculation for ExitOnNextEntry mode.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC8531D-AF18-44A0-97B5-62CB905615AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4594C634-4BF2-4417-89C8-E763EDA8BFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="1365" windowWidth="18315" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12510" yWindow="1965" windowWidth="20505" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -567,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="9">
-        <v>44228</v>
+        <v>44562</v>
       </c>
       <c r="E2" s="9">
         <v>44620</v>
@@ -647,16 +647,16 @@
         <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="H2" s="6">
-        <v>1.25</v>
+        <v>0.9</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>40</v>
@@ -908,56 +908,8 @@
       <c r="F43"/>
       <c r="I43"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44"/>
-      <c r="F44"/>
-      <c r="I44"/>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45"/>
-      <c r="F45"/>
-      <c r="I45"/>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="C46"/>
-      <c r="F46"/>
-      <c r="I46"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="C47"/>
-      <c r="F47"/>
-      <c r="I47"/>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="C48"/>
-      <c r="F48"/>
-      <c r="I48"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-      <c r="C49"/>
-      <c r="F49"/>
-      <c r="I49"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50"/>
-      <c r="F50"/>
-      <c r="I50"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51"/>
-      <c r="F51"/>
-      <c r="I51"/>
-    </row>
   </sheetData>
-  <dataValidations xWindow="923" yWindow="287" count="3">
+  <dataValidations xWindow="923" yWindow="287" count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman this option will override ADX_THRESHOLD field found in the class" sqref="L2:L1048576" xr:uid="{7257D8D3-A242-49AD-A664-6AC115EC7B9B}">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -966,9 +918,13 @@
       <formula1>1</formula1>
       <formula2>99999</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 H2:H1048576" xr:uid="{FC39107B-6731-40C3-900C-0A06F0710416}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H1048576" xr:uid="{FC39107B-6731-40C3-900C-0A06F0710416}">
       <formula1>0</formula1>
       <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E1048576" xr:uid="{A9F52B66-FA65-4A63-B461-7F30B13E5BAA}">
+      <formula1>36526</formula1>
+      <formula2>47484</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added StrategySettings dictionary support in TestCases.xlsx.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4594C634-4BF2-4417-89C8-E763EDA8BFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA15B66-4820-4631-A7E8-4674E6E6BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="1965" windowWidth="20505" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6930" yWindow="3750" windowWidth="24720" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ListOfValues" sheetId="2" r:id="rId2"/>
+    <sheet name="StrategyDictionaries" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Interval</t>
   </si>
@@ -151,14 +152,32 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>Option2</t>
+    <t>MACD:</t>
+  </si>
+  <si>
+    <t>Optional Strategy Settings</t>
+  </si>
+  <si>
+    <t>{"EMA": 200, "MACD_FAST": 12, "MACD_SLOW": 26, "MACD_SIGNAL": 9}</t>
+  </si>
+  <si>
+    <t>ScalpEmaRsiAdx:</t>
+  </si>
+  <si>
+    <t>{"EMA": 50, "EMA_TOLERANCE": 0, "RSI": 2, "RSI_MIN_SIGNAL": 20, "RSI_MAX_SIGNAL": 80, "RSI_MIN_ENTRY": 30, "RSI_MAX_ENTRY": 70, "ADX": 2, "ADX_THRESHOLD": 30, "CONFIRM_FILTER": false}</t>
+  </si>
+  <si>
+    <t>{"MA_TYPE": "SMA", "MACD_FAST": 2, "MACD_SLOW": 11, "BB_PERIODS": 40, "BB_MULT": 2, "ADX": 3, "ADX_THRESHOLD": 30}</t>
+  </si>
+  <si>
+    <t>MACD_BB_Freeman:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +192,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -240,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -287,6 +317,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,11 +623,10 @@
     <col min="8" max="8" width="8.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="184.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>5</v>
       </c>
@@ -620,14 +657,11 @@
       <c r="J1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -647,100 +681,125 @@
         <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="H2" s="6">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3"/>
-      <c r="F3"/>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="9">
+        <v>44562</v>
+      </c>
+      <c r="E3" s="9">
+        <v>44620</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4"/>
       <c r="F4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5"/>
       <c r="F5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6"/>
       <c r="F6"/>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7"/>
       <c r="F7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8"/>
       <c r="F8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9"/>
       <c r="F9"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10"/>
       <c r="F10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11"/>
       <c r="F11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12"/>
       <c r="F12"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13"/>
       <c r="F13"/>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14"/>
       <c r="F14"/>
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15"/>
       <c r="F15"/>
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16"/>
       <c r="F16"/>
@@ -909,11 +968,7 @@
       <c r="I43"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="923" yWindow="287" count="4">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman this option will override ADX_THRESHOLD field found in the class" sqref="L2:L1048576" xr:uid="{7257D8D3-A242-49AD-A664-6AC115EC7B9B}">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
-    </dataValidation>
+  <dataValidations xWindow="923" yWindow="287" count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{D812B71D-FF2F-483A-9C34-CCCA6DC36707}">
       <formula1>1</formula1>
       <formula2>99999</formula2>
@@ -926,12 +981,14 @@
       <formula1>36526</formula1>
       <formula2>47484</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Strategy Settings" prompt="Use a dictionary to specify the desired settings, order has no importance." sqref="K1" xr:uid="{1AFE61E0-E410-4E0F-AD97-02560A09D511}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Strategy Settings" prompt="Format  { &quot;key1&quot;: value1, &quot;key2&quot;: value2, … }" sqref="K2:K1048576" xr:uid="{28131E9F-8FA5-429B-A077-0E42CC401F15}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="923" yWindow="287" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="923" yWindow="287" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exchange" prompt="Please select exchange from dropdown list" xr:uid="{FDA4A053-4AB0-48B0-9CA3-6E8174E0D4D6}">
           <x14:formula1>
             <xm:f>ListOfValues!$A$2:$A$5</xm:f>
@@ -962,12 +1019,6 @@
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Parameter" prompt="For MACD_BB_Freeman this value will override the MA_CALCULATION_TYPE field in the class" xr:uid="{96A1433D-0EEB-474D-93F6-A823D5795C69}">
-          <x14:formula1>
-            <xm:f>ListOfValues!$F$2:$F$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -979,7 +1030,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,4 +1217,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2AEDE-8D0A-4F0F-8D7B-61A3C304761D}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="217.28515625" style="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed 1st draft of process_trades() using no loop.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA15B66-4820-4631-A7E8-4674E6E6BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E735E-0BF0-41CF-917B-D068880A5C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6930" yWindow="3750" windowWidth="24720" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4980" windowWidth="30300" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Interval</t>
   </si>
@@ -167,10 +167,10 @@
     <t>{"EMA": 50, "EMA_TOLERANCE": 0, "RSI": 2, "RSI_MIN_SIGNAL": 20, "RSI_MAX_SIGNAL": 80, "RSI_MIN_ENTRY": 30, "RSI_MAX_ENTRY": 70, "ADX": 2, "ADX_THRESHOLD": 30, "CONFIRM_FILTER": false}</t>
   </si>
   <si>
-    <t>{"MA_TYPE": "SMA", "MACD_FAST": 2, "MACD_SLOW": 11, "BB_PERIODS": 40, "BB_MULT": 2, "ADX": 3, "ADX_THRESHOLD": 30}</t>
-  </si>
-  <si>
     <t>MACD_BB_Freeman:</t>
+  </si>
+  <si>
+    <t>{"MA_TYPE": "SMA", "MACD_FAST": 2, "MACD_SLOW": 11, "BB_PERIODS": 40, "BB_MULT": 2, "ADX": 3, "ADX_THRESHOLD": 0}</t>
   </si>
 </sst>
 </file>
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +672,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="9">
-        <v>44562</v>
+        <v>44470</v>
       </c>
       <c r="E2" s="9">
         <v>44620</v>
@@ -692,40 +692,15 @@
       <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="9">
-        <v>44562</v>
-      </c>
-      <c r="E3" s="9">
-        <v>44620</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="15"/>
+      <c r="B3" s="1"/>
+      <c r="C3"/>
+      <c r="F3"/>
+      <c r="I3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -961,14 +936,9 @@
       <c r="F42"/>
       <c r="I42"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43"/>
-      <c r="F43"/>
-      <c r="I43"/>
-    </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Strategy Settings" prompt="Use a dictionary to specify the desired settings, order has no importance." sqref="K1" xr:uid="{1AFE61E0-E410-4E0F-AD97-02560A09D511}"/>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{D812B71D-FF2F-483A-9C34-CCCA6DC36707}">
       <formula1>1</formula1>
       <formula2>99999</formula2>
@@ -981,7 +951,6 @@
       <formula1>36526</formula1>
       <formula2>47484</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Strategy Settings" prompt="Use a dictionary to specify the desired settings, order has no importance." sqref="K1" xr:uid="{1AFE61E0-E410-4E0F-AD97-02560A09D511}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Optional Strategy Settings" prompt="Format  { &quot;key1&quot;: value1, &quot;key2&quot;: value2, … }" sqref="K2:K1048576" xr:uid="{28131E9F-8FA5-429B-A077-0E42CC401F15}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1224,7 +1193,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,10 +1220,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug where prev_row in process_trades() was not being reset between tests.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6E735E-0BF0-41CF-917B-D068880A5C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C3C293-BDB6-4C3A-9452-54DFCC675FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4980" windowWidth="30300" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="4755" windowWidth="26850" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" activeCellId="2" sqref="A3:XFD3 A4:XFD4 A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
     <col min="8" max="8" width="8.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="184.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="112.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -672,10 +672,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="9">
-        <v>44470</v>
+        <v>44562</v>
       </c>
       <c r="E2" s="9">
-        <v>44620</v>
+        <v>44594</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
@@ -697,22 +697,13 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3"/>
-      <c r="F3"/>
-      <c r="I3"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4"/>
-      <c r="F4"/>
-      <c r="I4"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5"/>
-      <c r="F5"/>
-      <c r="I5"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -923,18 +914,6 @@
       <c r="C40"/>
       <c r="F40"/>
       <c r="I40"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41"/>
-      <c r="F41"/>
-      <c r="I41"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="C42"/>
-      <c r="F42"/>
-      <c r="I42"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">

</xml_diff>

<commit_message>
Reverted to old version of find_entries() for ScalpEmaRsiAdx.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7972DAC5-BBF9-4BB7-A6B8-07022AF57EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A48E950-CCEF-4669-BE57-B91D25D1A30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11085" yWindow="3210" windowWidth="26850" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="3045" windowWidth="26850" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Interval</t>
   </si>
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,22 +672,22 @@
         <v>25</v>
       </c>
       <c r="D2" s="9">
-        <v>44197</v>
+        <v>44562</v>
       </c>
       <c r="E2" s="9">
-        <v>44561</v>
+        <v>44926</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="H2" s="6">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>34</v>
@@ -705,157 +705,51 @@
         <v>25</v>
       </c>
       <c r="D3" s="9">
-        <v>44197</v>
+        <v>44562</v>
       </c>
       <c r="E3" s="9">
-        <v>44561</v>
+        <v>44926</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="H3" s="6">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="K3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E4" s="9">
-        <v>44561</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E5" s="9">
-        <v>44561</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="H5" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="15"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4"/>
+      <c r="F4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5"/>
+      <c r="F5"/>
+      <c r="I5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E6" s="9">
-        <v>44561</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="H6" s="6">
-        <v>1.3</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6"/>
+      <c r="F6"/>
+      <c r="I6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E7" s="9">
-        <v>44561</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="H7" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7"/>
+      <c r="F7"/>
+      <c r="I7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -988,30 +882,6 @@
       <c r="C29"/>
       <c r="F29"/>
       <c r="I29"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30"/>
-      <c r="F30"/>
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31"/>
-      <c r="F31"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32"/>
-      <c r="F32"/>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33"/>
-      <c r="F33"/>
-      <c r="I33"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">

</xml_diff>

<commit_message>
Shortedned strategy details output.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A48E950-CCEF-4669-BE57-B91D25D1A30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FF5E39-8162-432E-9174-E9209F359728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="3045" windowWidth="26850" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5355" yWindow="900" windowWidth="26850" windowHeight="10125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Interval</t>
   </si>
@@ -608,7 +608,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +672,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="9">
-        <v>44562</v>
+        <v>44531</v>
       </c>
       <c r="E2" s="9">
         <v>44926</v>
@@ -681,10 +681,10 @@
         <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H2" s="6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>29</v>
@@ -695,121 +695,7 @@
       <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="9">
-        <v>44562</v>
-      </c>
-      <c r="E3" s="9">
-        <v>44926</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4"/>
-      <c r="F4"/>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5"/>
-      <c r="F5"/>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6"/>
-      <c r="F6"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7"/>
-      <c r="F7"/>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8"/>
-      <c r="F8"/>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9"/>
-      <c r="F9"/>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10"/>
-      <c r="F10"/>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11"/>
-      <c r="F11"/>
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12"/>
-      <c r="F12"/>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13"/>
-      <c r="F13"/>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14"/>
-      <c r="F14"/>
-      <c r="I14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15"/>
-      <c r="F15"/>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16"/>
-      <c r="F16"/>
-      <c r="I16"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17"/>
-      <c r="F17"/>
-      <c r="I17"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>

</xml_diff>

<commit_message>
Fixed error in dictionary provided in the TestCases.xlsx file.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1892E45C-647A-4B56-9B3B-59C088627D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72013A4-4218-408F-936B-546B8A5E9C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="4800" windowWidth="20070" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="4800" windowWidth="29790" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Interval</t>
   </si>
@@ -179,7 +179,7 @@
     <t>UtimateScalper:</t>
   </si>
   <si>
-    <t>{'EMA_Fast': 9, 'EMA_Slow': 55, 'EMA_Trend': 200, 'RSI': 2, 'RSI_Low': 48, 'RSI_High': 52, 'ADX': 14, 'ADX_Threshold': 0, 'MACD_Fast': 12, 'MACD_Slow': 26, 'MACD_Signal': 9, 'BB_Length': 34, 'BB_Mult': 1}</t>
+    <t>{"EMA_Fast": 9, "EMA_Slow": 55, "EMA_Trend": 200, "RSI": 2, "RSI_Low": 48, "RSI_High": 52, "ADX": 14, "ADX_Threshold": 0, "MACD_Fast": 12, "MACD_Slow": 26, "MACD_Signal": 9, "BB_Length": 34, "BB_Mult": 1}</t>
   </si>
 </sst>
 </file>
@@ -617,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,38 +706,11 @@
       </c>
       <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="9">
-        <v>44501</v>
-      </c>
-      <c r="E3" s="9">
-        <v>44926</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="15"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9"/>
+      <c r="F9"/>
+      <c r="I9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
@@ -804,12 +777,6 @@
       <c r="C20"/>
       <c r="F20"/>
       <c r="I20"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21"/>
-      <c r="F21"/>
-      <c r="I21"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">
@@ -1070,7 +1037,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added support for inverse perpetual and added code to validate data in db.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72013A4-4218-408F-936B-546B8A5E9C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FE1C4E-D6A3-4F9A-9EDB-FB5F8607172B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="4800" windowWidth="29790" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2025" yWindow="4110" windowWidth="25095" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Interval</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>{"EMA_Fast": 9, "EMA_Slow": 55, "EMA_Trend": 200, "RSI": 2, "RSI_Low": 48, "RSI_High": 52, "ADX": 14, "ADX_Threshold": 0, "MACD_Fast": 12, "MACD_Slow": 26, "MACD_Signal": 9, "BB_Length": 34, "BB_Mult": 1}</t>
+  </si>
+  <si>
+    <t>BTCUSD</t>
+  </si>
+  <si>
+    <t>ETHUSD</t>
   </si>
 </sst>
 </file>
@@ -617,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D2" s="9">
         <v>44501</v>
@@ -699,12 +705,18 @@
         <v>0.8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -771,12 +783,6 @@
       <c r="C19"/>
       <c r="F19"/>
       <c r="I19"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20"/>
-      <c r="F20"/>
-      <c r="I20"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">
@@ -841,7 +847,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +929,9 @@
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>39</v>
       </c>
@@ -937,7 +945,9 @@
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F5" s="5" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Fixed inversed condition in UltimateScalper.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FE1C4E-D6A3-4F9A-9EDB-FB5F8607172B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A41E897-4C9D-41A5-BF88-13984CF1D4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2025" yWindow="4110" windowWidth="25095" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Interval</t>
   </si>
@@ -626,7 +626,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,25 +687,25 @@
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D2" s="9">
-        <v>44501</v>
+        <v>44197</v>
       </c>
       <c r="E2" s="9">
         <v>44926</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="H2" s="6">
         <v>0.8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>34</v>
@@ -713,10 +713,103 @@
       <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="9">
+        <v>44197</v>
+      </c>
+      <c r="E3" s="9">
+        <v>44926</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="9">
+        <v>44197</v>
+      </c>
+      <c r="E4" s="9">
+        <v>44926</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="9">
+        <v>44197</v>
+      </c>
+      <c r="E5" s="9">
+        <v>44926</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>

<commit_message>
Fixed setting in UltimateScalper.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A41E897-4C9D-41A5-BF88-13984CF1D4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2830B4-C9F8-4145-B956-3EBBDA0AFD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="4110" windowWidth="25095" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="450" windowWidth="29835" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Interval</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>ETHUSD</t>
+  </si>
+  <si>
+    <t>Bybit_Testnet</t>
+  </si>
+  <si>
+    <t>{"EMA_Fast": 9, "EMA_Slow": 55, "EMA_Trend": 200, "RSI": 4, "RSI_Low": 19, "RSI_High": 81, "ADX": 17, "ADX_Threshold": 24, "MACD_Fast": 12, "MACD_Slow": 24, "MACD_Signal": 9, "BB_Length": 34, "BB_Mult": 1}</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +696,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="9">
-        <v>44197</v>
+        <v>44593</v>
       </c>
       <c r="E2" s="9">
         <v>44926</v>
@@ -710,106 +716,27 @@
       <c r="J2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E3" s="9">
-        <v>44926</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E4" s="9">
-        <v>44926</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="9">
-        <v>44197</v>
-      </c>
-      <c r="E5" s="9">
-        <v>44926</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="15"/>
+      <c r="K2" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6"/>
+      <c r="F6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7"/>
+      <c r="F7"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8"/>
+      <c r="F8"/>
+      <c r="I8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
@@ -858,24 +785,6 @@
       <c r="C16"/>
       <c r="F16"/>
       <c r="I16"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17"/>
-      <c r="F17"/>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18"/>
-      <c r="F18"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19"/>
-      <c r="F19"/>
-      <c r="I19"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">
@@ -940,7 +849,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +923,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
@@ -1139,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2AEDE-8D0A-4F0F-8D7B-61A3C304761D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed policy when sl/tp happen in the same candle.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2830B4-C9F8-4145-B956-3EBBDA0AFD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE81DA3D-296A-4A3D-BAB8-D4F9CA6A91E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="450" windowWidth="29835" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6690" yWindow="2775" windowWidth="27615" windowHeight="6675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Interval</t>
   </si>
@@ -186,18 +186,15 @@
   </si>
   <si>
     <t>ETHUSD</t>
-  </si>
-  <si>
-    <t>Bybit_Testnet</t>
-  </si>
-  <si>
-    <t>{"EMA_Fast": 9, "EMA_Slow": 55, "EMA_Trend": 200, "RSI": 4, "RSI_Low": 19, "RSI_High": 81, "ADX": 17, "ADX_Threshold": 24, "MACD_Fast": 12, "MACD_Slow": 24, "MACD_Signal": 9, "BB_Length": 34, "BB_Mult": 1}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,9 +303,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -348,6 +342,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -629,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,48 +640,48 @@
     <col min="1" max="1" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8" style="21" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="21" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="157.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="20" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -695,20 +695,20 @@
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="9">
-        <v>44593</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="D2" s="8">
+        <v>44197</v>
+      </c>
+      <c r="E2" s="8">
         <v>44926</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0.8</v>
+      <c r="G2" s="21">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H2" s="21">
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>48</v>
@@ -716,9 +716,16 @@
       <c r="J2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
@@ -773,18 +780,6 @@
       <c r="C14"/>
       <c r="F14"/>
       <c r="I14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15"/>
-      <c r="F15"/>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16"/>
-      <c r="F16"/>
-      <c r="I16"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">
@@ -849,24 +844,24 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="1"/>
     <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -878,18 +873,18 @@
       <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -898,18 +893,18 @@
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -918,18 +913,16 @@
       <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
@@ -941,11 +934,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
@@ -957,11 +950,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
@@ -969,11 +962,11 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
@@ -981,9 +974,9 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="5" t="s">
         <v>18</v>
       </c>
@@ -991,9 +984,9 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="5" t="s">
         <v>19</v>
       </c>
@@ -1001,9 +994,9 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1011,9 +1004,9 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1021,9 +1014,9 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
@@ -1031,9 +1024,9 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
@@ -1056,39 +1049,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="242.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="242.140625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created new strategy HA_VWAP.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331BE33F-BC9C-46ED-B995-D7E4B74310E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EAEFC4-EEC3-4C9B-B845-9268F7983DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="2775" windowWidth="24765" windowHeight="6735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6690" yWindow="2775" windowWidth="28845" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Interval</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>ETHUSD</t>
+  </si>
+  <si>
+    <t>VWAP_Touch</t>
+  </si>
+  <si>
+    <t>HA_VWAP</t>
+  </si>
+  <si>
+    <t>HA_VWAP:</t>
+  </si>
+  <si>
+    <t>{'EMA': 200', 'DistVWAP_PCT': 0.05', 'NB_SIGNALS': 2}</t>
   </si>
 </sst>
 </file>
@@ -193,7 +205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -632,7 +644,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,29 +708,59 @@
         <v>25</v>
       </c>
       <c r="D2" s="8">
-        <v>44470</v>
+        <v>44562</v>
       </c>
       <c r="E2" s="8">
         <v>44926</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="21">
-        <v>6.0000000000000001E-3</v>
+        <v>7</v>
       </c>
       <c r="H2" s="21">
-        <v>6.0000000000000001E-3</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8">
+        <v>44562</v>
+      </c>
+      <c r="E3" s="8">
+        <v>44926</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="21">
+        <v>7</v>
+      </c>
+      <c r="H3" s="21">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -811,7 +853,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strategy" prompt="Please select strategy from dropdown list" xr:uid="{46A140AA-8190-4C69-86E3-B269F7CB5240}">
           <x14:formula1>
-            <xm:f>ListOfValues!$B$2:$B$7</xm:f>
+            <xm:f>ListOfValues!$B$2:$B$8</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
@@ -829,7 +871,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Exit Strategy" prompt="Please select the way trades exit from the dropdown list" xr:uid="{3B7B2715-8F43-4FA9-A6F2-16C54D666CE1}">
           <x14:formula1>
-            <xm:f>ListOfValues!$C$2:$C$3</xm:f>
+            <xm:f>ListOfValues!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
@@ -844,7 +886,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +924,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>34</v>
@@ -920,9 +962,11 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
@@ -936,7 +980,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="5" t="s">
@@ -952,7 +996,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
@@ -964,7 +1008,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="5" t="s">
@@ -975,7 +1019,9 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="C8" s="7"/>
       <c r="D8" s="5" t="s">
         <v>18</v>
@@ -1034,6 +1080,9 @@
       <c r="F13" s="5"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B8">
+    <sortCondition ref="B2:B8"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1041,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2AEDE-8D0A-4F0F-8D7B-61A3C304761D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,6 +1134,14 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed error in tp/sl for HA_VWAP that created astronomical gains.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F48749-DF65-499A-B683-D1578B67F94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38EE72B-07DF-42FC-9F65-6B7D18F14860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="2775" windowWidth="28845" windowHeight="13605" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6690" yWindow="2775" windowWidth="28845" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Interval</t>
   </si>
@@ -197,10 +197,13 @@
     <t>HA_VWAP:</t>
   </si>
   <si>
-    <t>{"EMA": 200, "DistVWAP_PCT": 0.0, "NB_SIGNALS": 2}</t>
-  </si>
-  <si>
     <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 2}</t>
+  </si>
+  <si>
+    <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 1}</t>
+  </si>
+  <si>
+    <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 3}</t>
   </si>
 </sst>
 </file>
@@ -646,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +735,7 @@
         <v>53</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -767,26 +770,148 @@
         <v>53</v>
       </c>
       <c r="K3" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="8">
+        <v>44562</v>
+      </c>
+      <c r="E4" s="8">
+        <v>44926</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="21">
+        <v>7</v>
+      </c>
+      <c r="H4" s="21">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8">
+        <v>44562</v>
+      </c>
+      <c r="E5" s="8">
+        <v>44926</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="21">
+        <v>7</v>
+      </c>
+      <c r="H5" s="21">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K4" s="14"/>
-    </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6"/>
-      <c r="F6"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7"/>
-      <c r="F7"/>
-      <c r="I7"/>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8">
+        <v>44562</v>
+      </c>
+      <c r="E6" s="8">
+        <v>44926</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="21">
+        <v>7</v>
+      </c>
+      <c r="H6" s="21">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8">
+        <v>44562</v>
+      </c>
+      <c r="E7" s="8">
+        <v>44926</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="21">
+        <v>7</v>
+      </c>
+      <c r="H7" s="21">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -1099,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2AEDE-8D0A-4F0F-8D7B-61A3C304761D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1146,7 +1271,7 @@
         <v>55</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added NB_SIGNLAS=4 for HA_VWAP.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38EE72B-07DF-42FC-9F65-6B7D18F14860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC76083-77C6-42ED-BF87-9E7260148434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6690" yWindow="2775" windowWidth="28845" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>Interval</t>
   </si>
@@ -200,10 +200,10 @@
     <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 2}</t>
   </si>
   <si>
-    <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 1}</t>
-  </si>
-  <si>
-    <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 3}</t>
+    <t>{"EMA": 200, "DistVWAP_PCT": 0.0, "NB_SIGNALS": 3}</t>
+  </si>
+  <si>
+    <t>{"EMA": 200, "DistVWAP_PCT": 0.0, "NB_SIGNALS": 4}</t>
   </si>
 </sst>
 </file>
@@ -647,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
@@ -770,190 +770,38 @@
         <v>53</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="8">
-        <v>44562</v>
-      </c>
-      <c r="E4" s="8">
-        <v>44926</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="21">
-        <v>7</v>
-      </c>
-      <c r="H4" s="21">
-        <v>7</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8">
-        <v>44562</v>
-      </c>
-      <c r="E5" s="8">
-        <v>44926</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="21">
-        <v>7</v>
-      </c>
-      <c r="H5" s="21">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="8">
-        <v>44562</v>
-      </c>
-      <c r="E6" s="8">
-        <v>44926</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="21">
-        <v>7</v>
-      </c>
-      <c r="H6" s="21">
-        <v>7</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="8">
-        <v>44562</v>
-      </c>
-      <c r="E7" s="8">
-        <v>44926</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="21">
-        <v>7</v>
-      </c>
-      <c r="H7" s="21">
-        <v>7</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>58</v>
-      </c>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4"/>
+      <c r="F4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5"/>
+      <c r="F5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6"/>
+      <c r="F6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7"/>
+      <c r="F7"/>
+      <c r="I7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8"/>
       <c r="F8"/>
       <c r="I8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9"/>
-      <c r="F9"/>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10"/>
-      <c r="F10"/>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11"/>
-      <c r="F11"/>
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12"/>
-      <c r="F12"/>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13"/>
-      <c r="F13"/>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14"/>
-      <c r="F14"/>
-      <c r="I14"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">

</xml_diff>

<commit_message>
Added parameter to HA_VWAP strategy.
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Learning\Trading\BackTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC76083-77C6-42ED-BF87-9E7260148434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B2ECE7-288E-4F64-BEAF-98188E50CF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="2775" windowWidth="28845" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="0" windowWidth="21195" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Interval</t>
   </si>
@@ -197,13 +197,7 @@
     <t>HA_VWAP:</t>
   </si>
   <si>
-    <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "NB_SIGNALS": 2}</t>
-  </si>
-  <si>
-    <t>{"EMA": 200, "DistVWAP_PCT": 0.0, "NB_SIGNALS": 3}</t>
-  </si>
-  <si>
-    <t>{"EMA": 200, "DistVWAP_PCT": 0.0, "NB_SIGNALS": 4}</t>
+    <t>{"EMA": 200, "DistVWAP_PCT": 0.05, "Nb_Signals": 2, "ExitOnEmaCross": false}</t>
   </si>
 </sst>
 </file>
@@ -647,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +714,7 @@
         <v>44926</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="21">
         <v>7</v>
@@ -734,19 +728,17 @@
       <c r="J2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>57</v>
-      </c>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="8">
         <v>44562</v>
@@ -755,7 +747,7 @@
         <v>44926</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="21">
         <v>7</v>
@@ -769,9 +761,7 @@
       <c r="J3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>58</v>
-      </c>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -796,12 +786,6 @@
       <c r="C7"/>
       <c r="F7"/>
       <c r="I7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8"/>
-      <c r="F8"/>
-      <c r="I8"/>
     </row>
   </sheetData>
   <dataValidations xWindow="923" yWindow="287" count="5">
@@ -1072,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2AEDE-8D0A-4F0F-8D7B-61A3C304761D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>